<commit_message>
Week 5 (ongoing with some changes)
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A7E12F-CDED-4F48-929B-3A3BDE8B1720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA968CB7-615B-AC45-9DAE-02AEC3F589C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="134">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>Figma Layout for design v2, to be displayed in client meet 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-01-24: Need to write a misson statement, divide team into frontend and backend. </t>
   </si>
 </sst>
 </file>
@@ -1399,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -1882,8 +1885,8 @@
       <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>54</v>
+      <c r="C22" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -1911,7 +1914,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
@@ -2015,6 +2018,9 @@
       <c r="F26" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="G26" s="39" t="s">
+        <v>133</v>
+      </c>
       <c r="H26" s="12">
         <f t="shared" si="0"/>
         <v>-0.5</v>
@@ -2032,7 +2038,7 @@
         <v>44</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -2195,7 +2201,7 @@
       <c r="F33" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="33" t="s">
         <v>101</v>
       </c>
       <c r="H33" s="12">
@@ -2226,7 +2232,7 @@
       <c r="F34" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="33" t="s">
         <v>102</v>
       </c>
       <c r="H34" s="12">
@@ -2257,7 +2263,7 @@
       <c r="F35" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="33" t="s">
         <v>103</v>
       </c>
       <c r="H35" s="12">
@@ -2288,7 +2294,7 @@
       <c r="F36" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="33" t="s">
         <v>110</v>
       </c>
       <c r="H36" s="12">
@@ -2308,7 +2314,7 @@
         <v>44</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
@@ -2319,7 +2325,7 @@
       <c r="F37" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="33" t="s">
         <v>111</v>
       </c>
       <c r="H37" s="12">
@@ -2350,7 +2356,7 @@
       <c r="F38" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="33" t="s">
         <v>104</v>
       </c>
       <c r="H38" s="12">
@@ -2379,7 +2385,7 @@
       <c r="F39" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="33" t="s">
         <v>108</v>
       </c>
       <c r="H39" s="12">
@@ -2410,7 +2416,7 @@
       <c r="F40" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="33" t="s">
         <v>109</v>
       </c>
       <c r="H40" s="12">
@@ -2438,7 +2444,7 @@
       <c r="F41" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="33" t="s">
         <v>105</v>
       </c>
       <c r="H41" s="12"/>
@@ -2460,7 +2466,7 @@
       <c r="F42" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="33" t="s">
         <v>106</v>
       </c>
       <c r="H42" s="12"/>
@@ -2482,7 +2488,7 @@
       <c r="F43" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="33" t="s">
         <v>107</v>
       </c>
       <c r="H43" s="12" t="str">

</xml_diff>

<commit_message>
Week 6 Planned, Week 5 completed
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1118AFA2-901A-F446-B555-B9BB6641080C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{226550C8-9778-0846-826D-E3C8F91AD1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="1180" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="151">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -349,9 +349,6 @@
     <t>Week 3 (January 29 - February 4)</t>
   </si>
   <si>
-    <t>Week 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Team Meeting </t>
   </si>
   <si>
@@ -542,6 +539,54 @@
   </si>
   <si>
     <t>Cloud Services Alternatives</t>
+  </si>
+  <si>
+    <t>Client meeting-11</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-11</t>
+  </si>
+  <si>
+    <t>SRS Document v1</t>
+  </si>
+  <si>
+    <t>Test Plan Tracker v1</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to discuss what to include in SRS and how to start with the coding aspects of the project </t>
+  </si>
+  <si>
+    <t>Week 6 (February 21 - February 28)</t>
+  </si>
+  <si>
+    <t>16-02-24: Discussed about inputs on the task bar below, and keep multiple versions in handy for items page and home page. Start coding of these two pages.</t>
+  </si>
+  <si>
+    <t>Client meeting-12</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-12</t>
+  </si>
+  <si>
+    <t>Client meeting-13</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-13</t>
+  </si>
+  <si>
+    <t>Implementation-Home Page</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Implementation-Items Page</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -688,7 +733,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -790,9 +835,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -912,10 +954,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1406,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I262"/>
+  <dimension ref="A1:I267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -1506,11 +1544,11 @@
       <c r="F7" s="15"/>
       <c r="G7" s="2"/>
       <c r="H7" s="12" t="str">
-        <f t="shared" ref="H7:H99" si="0">IF(OR(D7="", E7=""), "", D7-E7)</f>
+        <f t="shared" ref="H7:H104" si="0">IF(OR(D7="", E7=""), "", D7-E7)</f>
         <v/>
       </c>
       <c r="I7" s="12" t="str">
-        <f t="shared" ref="I7:I99" si="1">IF(OR(H7="",E7=0),"",ABS(H7)/E7*100)</f>
+        <f t="shared" ref="I7:I104" si="1">IF(OR(H7="",E7=0),"",ABS(H7)/E7*100)</f>
         <v/>
       </c>
     </row>
@@ -1914,7 +1952,7 @@
     </row>
     <row r="23" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A23" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
@@ -1932,7 +1970,7 @@
         <v>41</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H23" s="12">
         <f t="shared" si="0"/>
@@ -1976,7 +2014,7 @@
     </row>
     <row r="25" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A25" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
@@ -1994,7 +2032,7 @@
         <v>41</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H25" s="12">
         <f t="shared" si="0"/>
@@ -2007,7 +2045,7 @@
     </row>
     <row r="26" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A26" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
@@ -2024,8 +2062,8 @@
       <c r="F26" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="39" t="s">
-        <v>132</v>
+      <c r="G26" s="33" t="s">
+        <v>131</v>
       </c>
       <c r="H26" s="12">
         <f t="shared" si="0"/>
@@ -2038,7 +2076,7 @@
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A27" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
@@ -2082,7 +2120,7 @@
         <v>55</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H28" s="12" t="str">
         <f t="shared" si="0"/>
@@ -2123,7 +2161,7 @@
     </row>
     <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
@@ -2138,14 +2176,14 @@
         <v>55</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>44</v>
@@ -2160,7 +2198,7 @@
         <v>55</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H31" s="12" t="str">
         <f t="shared" si="0"/>
@@ -2208,7 +2246,7 @@
         <v>51</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H33" s="12">
         <f t="shared" ref="H33:H34" si="2">IF(OR(D33="", E33=""), "", D33-E33)</f>
@@ -2221,7 +2259,7 @@
     </row>
     <row r="34" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="36" t="s">
         <v>38</v>
@@ -2239,7 +2277,7 @@
         <v>51</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H34" s="12">
         <f t="shared" si="2"/>
@@ -2252,7 +2290,7 @@
     </row>
     <row r="35" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>44</v>
@@ -2270,7 +2308,7 @@
         <v>41</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H35" s="12">
         <f t="shared" ref="H35" si="4">IF(OR(D35="", E35=""), "", D35-E35)</f>
@@ -2283,7 +2321,7 @@
     </row>
     <row r="36" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="36" t="s">
         <v>35</v>
@@ -2301,7 +2339,7 @@
         <v>41</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H36" s="12">
         <f t="shared" ref="H36" si="6">IF(OR(D36="", E36=""), "", D36-E36)</f>
@@ -2314,7 +2352,7 @@
     </row>
     <row r="37" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="36" t="s">
         <v>44</v>
@@ -2332,7 +2370,7 @@
         <v>41</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H37" s="12">
         <f t="shared" ref="H37" si="8">IF(OR(D37="", E37=""), "", D37-E37)</f>
@@ -2345,7 +2383,7 @@
     </row>
     <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="36" t="s">
         <v>35</v>
@@ -2363,7 +2401,7 @@
         <v>41</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H38" s="12">
         <v>0</v>
@@ -2374,7 +2412,7 @@
     </row>
     <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>44</v>
@@ -2392,7 +2430,7 @@
         <v>41</v>
       </c>
       <c r="G39" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H39" s="12">
         <f t="shared" ref="H39" si="10">IF(OR(D39="", E39=""), "", D39-E39)</f>
@@ -2405,7 +2443,7 @@
     </row>
     <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="36" t="s">
         <v>35</v>
@@ -2423,7 +2461,7 @@
         <v>41</v>
       </c>
       <c r="G40" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H40" s="12">
         <f t="shared" ref="H40" si="12">IF(OR(D40="", E40=""), "", D40-E40)</f>
@@ -2436,7 +2474,7 @@
     </row>
     <row r="41" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="36" t="s">
         <v>38</v>
@@ -2451,17 +2489,17 @@
         <v>55</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="35" t="s">
         <v>45</v>
@@ -2473,17 +2511,17 @@
         <v>55</v>
       </c>
       <c r="G42" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" s="35" t="s">
         <v>40</v>
@@ -2495,7 +2533,7 @@
         <v>55</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H43" s="12" t="str">
         <f t="shared" si="0"/>
@@ -2508,7 +2546,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="4"/>
@@ -2527,7 +2565,7 @@
     </row>
     <row r="45" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="36" t="s">
         <v>38</v>
@@ -2545,7 +2583,7 @@
         <v>51</v>
       </c>
       <c r="G45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H45" s="12">
         <f t="shared" si="0"/>
@@ -2558,10 +2596,10 @@
     </row>
     <row r="46" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>54</v>
@@ -2576,7 +2614,7 @@
         <v>41</v>
       </c>
       <c r="G46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H46" s="12">
         <f>IF(OR(D46="", E46=""), "", D46-E46)</f>
@@ -2588,10 +2626,10 @@
     </row>
     <row r="47" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>40</v>
@@ -2606,7 +2644,7 @@
         <v>51</v>
       </c>
       <c r="G47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H47" s="12">
         <v>1</v>
@@ -2617,7 +2655,7 @@
     </row>
     <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="36" t="s">
         <v>35</v>
@@ -2635,7 +2673,7 @@
         <v>41</v>
       </c>
       <c r="G48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H48" s="12">
         <v>0</v>
@@ -2646,7 +2684,7 @@
     </row>
     <row r="49" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>44</v>
@@ -2672,7 +2710,7 @@
     </row>
     <row r="50" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="36" t="s">
         <v>35</v>
@@ -2690,7 +2728,7 @@
         <v>41</v>
       </c>
       <c r="G50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H50" s="12">
         <v>0</v>
@@ -2701,7 +2739,7 @@
     </row>
     <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>44</v>
@@ -2727,7 +2765,7 @@
     </row>
     <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="36" t="s">
         <v>44</v>
@@ -2746,10 +2784,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>47</v>
@@ -2771,7 +2809,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="10"/>
@@ -2790,7 +2828,7 @@
     </row>
     <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
         <v>44</v>
@@ -2807,8 +2845,8 @@
       <c r="F55" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G55" s="39" t="s">
-        <v>124</v>
+      <c r="G55" s="33" t="s">
+        <v>123</v>
       </c>
       <c r="H55" s="12">
         <f t="shared" si="0"/>
@@ -2821,10 +2859,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="35" t="s">
         <v>45</v>
@@ -2838,8 +2876,8 @@
       <c r="F56" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G56" s="40" t="s">
-        <v>125</v>
+      <c r="G56" s="39" t="s">
+        <v>124</v>
       </c>
       <c r="H56" s="12">
         <f t="shared" si="0"/>
@@ -2852,7 +2890,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="36" t="s">
         <v>35</v>
@@ -2869,8 +2907,8 @@
       <c r="F57" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G57" s="40" t="s">
-        <v>126</v>
+      <c r="G57" s="39" t="s">
+        <v>125</v>
       </c>
       <c r="H57" s="12">
         <v>0</v>
@@ -2881,7 +2919,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B58" s="36" t="s">
         <v>44</v>
@@ -2908,7 +2946,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A59" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B59" s="36" t="s">
         <v>35</v>
@@ -2925,8 +2963,8 @@
       <c r="F59" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G59" s="40" t="s">
-        <v>127</v>
+      <c r="G59" s="39" t="s">
+        <v>126</v>
       </c>
       <c r="H59" s="12">
         <v>0</v>
@@ -2937,7 +2975,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A60" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" s="36" t="s">
         <v>35</v>
@@ -2954,8 +2992,8 @@
       <c r="F60" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G60" s="40" t="s">
-        <v>133</v>
+      <c r="G60" s="39" t="s">
+        <v>132</v>
       </c>
       <c r="H60" s="12">
         <v>0</v>
@@ -2966,7 +3004,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" s="36" t="s">
         <v>44</v>
@@ -2995,10 +3033,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C62" s="35" t="s">
         <v>40</v>
@@ -3010,10 +3048,10 @@
         <v>2</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G62" s="40" t="s">
-        <v>128</v>
+        <v>41</v>
+      </c>
+      <c r="G62" s="39" t="s">
+        <v>127</v>
       </c>
       <c r="H62" s="12">
         <f t="shared" ref="H62" si="14">IF(OR(D62="", E62=""), "", D62-E62)</f>
@@ -3043,15 +3081,19 @@
       <c r="F63" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G63" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
+      <c r="G63" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="H63" s="12">
+        <v>0</v>
+      </c>
+      <c r="I63" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" t="s">
         <v>38</v>
@@ -3068,8 +3110,8 @@
       <c r="F64" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G64" s="39" t="s">
-        <v>123</v>
+      <c r="G64" s="33" t="s">
+        <v>122</v>
       </c>
       <c r="H64" s="12">
         <v>0</v>
@@ -3080,10 +3122,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C65" s="35" t="s">
         <v>45</v>
@@ -3097,8 +3139,8 @@
       <c r="F65" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G65" s="40" t="s">
-        <v>131</v>
+      <c r="G65" s="39" t="s">
+        <v>130</v>
       </c>
       <c r="H65" s="12">
         <v>0</v>
@@ -3109,10 +3151,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C66" s="35" t="s">
         <v>47</v>
@@ -3132,77 +3174,143 @@
         <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C67" s="35" t="s">
         <v>50</v>
       </c>
       <c r="D67" s="5">
+        <v>5</v>
+      </c>
+      <c r="E67" s="5">
+        <v>5</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G67" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H67" s="12">
+        <v>0</v>
+      </c>
+      <c r="I67" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A68" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" s="5">
+        <v>1</v>
+      </c>
+      <c r="E68" s="5">
+        <v>1</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G68" s="33"/>
+      <c r="H68" s="12">
+        <v>0</v>
+      </c>
+      <c r="I68" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A69" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" s="5">
+        <v>4</v>
+      </c>
+      <c r="E69" s="5">
+        <v>5</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H69" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I69" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A70" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D70" s="5">
+        <v>10</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" s="33"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A71" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" s="5">
         <v>3</v>
       </c>
-      <c r="F67" s="16" t="s">
+      <c r="F71" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G67" s="33"/>
-      <c r="H67" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I67" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A68" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I68" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H69" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I69" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H70" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I70" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H71" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I71" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="G71" s="33"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A72" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="5">
+        <v>3</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G72" s="33"/>
       <c r="H72" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3213,6 +3321,15 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="2"/>
       <c r="H73" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3223,26 +3340,56 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H74" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I74" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A74" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D74" s="5">
+        <v>5</v>
+      </c>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A75" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="5">
+        <v>10</v>
+      </c>
       <c r="H75" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(D75="", E74=""), "", D75-E74)</f>
         <v/>
       </c>
       <c r="I75" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(H75="",E74=0),"",ABS(H75)/E74*100)</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A76" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" t="s">
+        <v>139</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D76" s="5">
+        <v>3</v>
+      </c>
       <c r="H76" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3253,6 +3400,18 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A77" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="5">
+        <v>3</v>
+      </c>
       <c r="H77" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3263,6 +3422,18 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A78" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" s="5">
+        <v>5</v>
+      </c>
       <c r="H78" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3273,6 +3444,18 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A79" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C79" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="5">
+        <v>1</v>
+      </c>
       <c r="H79" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3283,6 +3466,18 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A80" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" s="5">
+        <v>5</v>
+      </c>
       <c r="H80" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3292,7 +3487,19 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A81" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D81" s="5">
+        <v>5</v>
+      </c>
       <c r="H81" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3302,7 +3509,19 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A82" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D82" s="5">
+        <v>1</v>
+      </c>
       <c r="H82" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3312,7 +3531,19 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A83" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B83" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" s="5">
+        <v>4</v>
+      </c>
       <c r="H83" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3322,7 +3553,19 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A84" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" t="s">
+        <v>148</v>
+      </c>
+      <c r="C84" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84" s="5">
+        <v>4</v>
+      </c>
       <c r="H84" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3332,9 +3575,21 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A85" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" s="5">
+        <v>3</v>
+      </c>
       <c r="H85" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(D85="", E85=""), "", D85-E85)</f>
         <v/>
       </c>
       <c r="I85" s="12" t="str">
@@ -3342,9 +3597,11 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A86" s="36"/>
+      <c r="C86" s="35"/>
       <c r="H86" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(D86="", E86=""), "", D86-E86)</f>
         <v/>
       </c>
       <c r="I86" s="12" t="str">
@@ -3352,7 +3609,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H87" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3362,7 +3619,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H88" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3372,7 +3629,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H89" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3382,7 +3639,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H90" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3392,7 +3649,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H91" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3402,7 +3659,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H92" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3412,7 +3669,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H93" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3422,7 +3679,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H94" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3432,7 +3689,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H95" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3442,7 +3699,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H96" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3484,61 +3741,61 @@
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H100" s="12" t="str">
-        <f t="shared" ref="H100:H163" si="16">IF(OR(D100="", E100=""), "", D100-E100)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I100" s="12" t="str">
-        <f t="shared" ref="I100:I163" si="17">IF(OR(H100="",E100=0),"",ABS(H100)/E100*100)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H101" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I101" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H102" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I102" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H103" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I103" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H104" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I104" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H105" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="H105:H168" si="16">IF(OR(D105="", E105=""), "", D105-E105)</f>
         <v/>
       </c>
       <c r="I105" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="I105:I168" si="17">IF(OR(H105="",E105=0),"",ABS(H105)/E105*100)</f>
         <v/>
       </c>
     </row>
@@ -4124,61 +4381,61 @@
     </row>
     <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="12" t="str">
-        <f t="shared" ref="H164:H227" si="18">IF(OR(D164="", E164=""), "", D164-E164)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I164" s="12" t="str">
-        <f t="shared" ref="I164:I227" si="19">IF(OR(H164="",E164=0),"",ABS(H164)/E164*100)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I165" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I166" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I167" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I168" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="H169:H232" si="18">IF(OR(D169="", E169=""), "", D169-E169)</f>
         <v/>
       </c>
       <c r="I169" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="I169:I232" si="19">IF(OR(H169="",E169=0),"",ABS(H169)/E169*100)</f>
         <v/>
       </c>
     </row>
@@ -4764,61 +5021,61 @@
     </row>
     <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H228" s="12" t="str">
-        <f t="shared" ref="H228:H255" si="20">IF(OR(D228="", E228=""), "", D228-E228)</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I228" s="12" t="str">
-        <f t="shared" ref="I228:I262" si="21">IF(OR(H228="",E228=0),"",ABS(H228)/E228*100)</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H229" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I229" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H230" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I230" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H231" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I231" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H232" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I232" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H233" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="H233:H260" si="20">IF(OR(D233="", E233=""), "", D233-E233)</f>
         <v/>
       </c>
       <c r="I233" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="I233:I267" si="21">IF(OR(H233="",E233=0),"",ABS(H233)/E233*100)</f>
         <v/>
       </c>
     </row>
@@ -5043,50 +5300,100 @@
       </c>
     </row>
     <row r="256" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H256" s="12" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
       <c r="I256" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
-    <row r="257" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="257" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H257" s="12" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
       <c r="I257" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
-    <row r="258" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="258" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H258" s="12" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
       <c r="I258" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
-    <row r="259" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="259" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H259" s="12" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
       <c r="I259" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
-    <row r="260" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="260" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H260" s="12" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
       <c r="I260" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
-    <row r="261" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="261" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I261" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
-    <row r="262" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="262" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I262" s="12" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
+    <row r="263" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I263" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="264" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I264" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="265" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I265" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="266" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I266" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="267" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I267" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="F5:F10 F12:F33 F35:F65542">
+  <conditionalFormatting sqref="F5:F10 F12:F33 F35:F65547">
     <cfRule type="cellIs" dxfId="2" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Delayed"</formula>
     </cfRule>
@@ -5098,10 +5405,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65542" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65547" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, Ongoing, Delayed, Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B58:B65542" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B58:B65547" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Requirements, Design, Development, Testing, Preparation, Coordination, Documentation, Interfaces, Delivery"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
week 6 almost done
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{226550C8-9778-0846-826D-E3C8F91AD1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BEDABE6-05EE-D84A-80D1-61245F9549CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1180" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="168">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -587,6 +587,57 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS v1 sent to client for approval, uploaded on github. </t>
+  </si>
+  <si>
+    <t>19-02-24: Final changes asked to be made in UI</t>
+  </si>
+  <si>
+    <t>20-01-24: Urgent meet called to discuss inputs on final design changes. Only need to implement Home Page, with major design changes</t>
+  </si>
+  <si>
+    <t>Client meeting-14</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-14</t>
+  </si>
+  <si>
+    <t>Delayed</t>
+  </si>
+  <si>
+    <t>Major design changes requested by client, possibility of not implementing this at all</t>
+  </si>
+  <si>
+    <t>Working on differences in costing as well as efficiency between Digital Ocean and AWS</t>
+  </si>
+  <si>
+    <t>Need to discuss how to proceeed with new client requirements, and accordingly start updating the docs</t>
+  </si>
+  <si>
+    <t>Need to implement the new home page</t>
+  </si>
+  <si>
+    <t>Submitted on 22-02-24 based on the updated requirements of client</t>
+  </si>
+  <si>
+    <t>SRS Document v2</t>
+  </si>
+  <si>
+    <t>We need to get confirmations from client on what they need to change for home page</t>
+  </si>
+  <si>
+    <t>Look into React Native, and Flask frameworks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Making changes to use cases, and user case description. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-02-24: </t>
+  </si>
+  <si>
+    <t>Week 7 (February 29 - March 6)</t>
   </si>
 </sst>
 </file>
@@ -733,7 +784,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -837,6 +888,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1446,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -3352,8 +3406,21 @@
       <c r="D74" s="5">
         <v>5</v>
       </c>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
+      <c r="E74" s="5">
+        <v>4</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G74" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="H74" s="12">
+        <v>1</v>
+      </c>
+      <c r="I74" s="12">
+        <v>25</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75" s="36" t="s">
@@ -3368,13 +3435,22 @@
       <c r="D75" s="5">
         <v>10</v>
       </c>
-      <c r="H75" s="12" t="str">
-        <f>IF(OR(D75="", E74=""), "", D75-E74)</f>
-        <v/>
-      </c>
-      <c r="I75" s="12" t="str">
-        <f>IF(OR(H75="",E74=0),"",ABS(H75)/E74*100)</f>
-        <v/>
+      <c r="E75" s="5">
+        <v>12</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G75" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="H75" s="12">
+        <f t="shared" ref="H75" si="16">IF(OR(D75="", E75=""), "", D75-E75)</f>
+        <v>-2</v>
+      </c>
+      <c r="I75" s="12">
+        <f t="shared" ref="I75" si="17">IF(OR(H75="",E75=0),"",ABS(H75)/E75*100)</f>
+        <v>16.666666666666664</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
@@ -3385,15 +3461,18 @@
         <v>139</v>
       </c>
       <c r="C76" s="35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D76" s="5">
         <v>3</v>
       </c>
-      <c r="H76" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F76" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G76" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="H76" s="12"/>
       <c r="I76" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3412,13 +3491,22 @@
       <c r="D77" s="5">
         <v>3</v>
       </c>
-      <c r="H77" s="12" t="str">
+      <c r="E77" s="5">
+        <v>2</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G77" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="H77" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I77" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="I77" s="12">
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.15">
@@ -3429,18 +3517,27 @@
         <v>35</v>
       </c>
       <c r="C78" s="35" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D78" s="5">
         <v>5</v>
       </c>
-      <c r="H78" s="12" t="str">
+      <c r="E78" s="5">
+        <v>5</v>
+      </c>
+      <c r="F78" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G78" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H78" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I78" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="I78" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.15">
@@ -3451,18 +3548,25 @@
         <v>44</v>
       </c>
       <c r="C79" s="35" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D79" s="5">
         <v>1</v>
       </c>
-      <c r="H79" s="12" t="str">
+      <c r="E79" s="5">
+        <v>1</v>
+      </c>
+      <c r="F79" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G79" s="33"/>
+      <c r="H79" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I79" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="I79" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.15">
@@ -3478,13 +3582,22 @@
       <c r="D80" s="5">
         <v>5</v>
       </c>
-      <c r="H80" s="12" t="str">
+      <c r="E80" s="5">
+        <v>5</v>
+      </c>
+      <c r="F80" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G80" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="H80" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I80" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="I80" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.15">
@@ -3495,18 +3608,27 @@
         <v>35</v>
       </c>
       <c r="C81" s="35" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D81" s="5">
         <v>5</v>
       </c>
-      <c r="H81" s="12" t="str">
+      <c r="E81" s="5">
+        <v>4</v>
+      </c>
+      <c r="F81" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G81" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H81" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I81" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="I81" s="12">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.15">
@@ -3522,13 +3644,20 @@
       <c r="D82" s="5">
         <v>1</v>
       </c>
-      <c r="H82" s="12" t="str">
+      <c r="E82" s="5">
+        <v>1</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G82" s="33"/>
+      <c r="H82" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I82" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="I82" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.15">
@@ -3544,6 +3673,12 @@
       <c r="D83" s="5">
         <v>4</v>
       </c>
+      <c r="F83" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G83" s="40" t="s">
+        <v>163</v>
+      </c>
       <c r="H83" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3566,6 +3701,12 @@
       <c r="D84" s="5">
         <v>4</v>
       </c>
+      <c r="F84" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G84" s="40" t="s">
+        <v>157</v>
+      </c>
       <c r="H84" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3588,18 +3729,40 @@
       <c r="D85" s="5">
         <v>3</v>
       </c>
-      <c r="H85" s="12" t="str">
+      <c r="E85" s="5">
+        <v>2</v>
+      </c>
+      <c r="F85" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G85" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H85" s="12">
         <f>IF(OR(D85="", E85=""), "", D85-E85)</f>
-        <v/>
-      </c>
-      <c r="I85" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="I85" s="12">
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A86" s="36"/>
-      <c r="C86" s="35"/>
+      <c r="A86" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D86" s="5">
+        <v>5</v>
+      </c>
+      <c r="G86" s="39" t="s">
+        <v>166</v>
+      </c>
       <c r="H86" s="12" t="str">
         <f>IF(OR(D86="", E86=""), "", D86-E86)</f>
         <v/>
@@ -3610,23 +3773,57 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A87" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" s="5">
+        <v>1</v>
+      </c>
+      <c r="G87" s="33"/>
       <c r="H87" s="12" t="str">
+        <f>IF(OR(D87="", E87=""), "", D87-E87)</f>
+        <v/>
+      </c>
+      <c r="I87" s="12" t="str">
+        <f>IF(OR(H87="",E87=0),"",ABS(H87)/E87*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A88" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B88" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88" s="5">
+        <v>5</v>
+      </c>
+      <c r="E88" s="5">
+        <v>2</v>
+      </c>
+      <c r="F88" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G88" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="H88" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I87" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H88" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I88" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="I88" s="12">
+        <f t="shared" si="1"/>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.15">
@@ -3660,6 +3857,15 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="2"/>
       <c r="H92" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3791,1603 +3997,1603 @@
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H105" s="12" t="str">
-        <f t="shared" ref="H105:H168" si="16">IF(OR(D105="", E105=""), "", D105-E105)</f>
+        <f t="shared" ref="H105:H168" si="18">IF(OR(D105="", E105=""), "", D105-E105)</f>
         <v/>
       </c>
       <c r="I105" s="12" t="str">
-        <f t="shared" ref="I105:I168" si="17">IF(OR(H105="",E105=0),"",ABS(H105)/E105*100)</f>
+        <f t="shared" ref="I105:I168" si="19">IF(OR(H105="",E105=0),"",ABS(H105)/E105*100)</f>
         <v/>
       </c>
     </row>
     <row r="106" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H106" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I106" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H107" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I107" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H108" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I108" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H109" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I109" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H110" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I110" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H111" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I111" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H112" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I112" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H113" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I113" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H114" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I114" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H115" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I115" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H116" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I116" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H117" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I117" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H118" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I118" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H119" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I119" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H120" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I120" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H121" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I121" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H122" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I122" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H123" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I123" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H124" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I124" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H125" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I125" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H126" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I126" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H127" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I127" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H128" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I128" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H129" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I129" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H130" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I130" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H131" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I131" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="132" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H132" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I132" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H133" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I133" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H134" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I134" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H135" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I135" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H136" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I136" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H137" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I137" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H138" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I138" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H139" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I139" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H140" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I140" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H141" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I141" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H142" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I142" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H143" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I143" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H144" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I144" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H145" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I145" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H146" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I146" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H147" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I147" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H148" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I148" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H149" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I149" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H150" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I150" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H151" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I151" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H152" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I152" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H153" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I153" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H154" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I154" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H155" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I155" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H156" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I156" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H157" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I157" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H158" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I158" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H159" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I159" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H160" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I160" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H161" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I161" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H162" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I162" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H163" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I163" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I164" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I165" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I166" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I167" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I168" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="12" t="str">
-        <f t="shared" ref="H169:H232" si="18">IF(OR(D169="", E169=""), "", D169-E169)</f>
+        <f t="shared" ref="H169:H232" si="20">IF(OR(D169="", E169=""), "", D169-E169)</f>
         <v/>
       </c>
       <c r="I169" s="12" t="str">
-        <f t="shared" ref="I169:I232" si="19">IF(OR(H169="",E169=0),"",ABS(H169)/E169*100)</f>
+        <f t="shared" ref="I169:I232" si="21">IF(OR(H169="",E169=0),"",ABS(H169)/E169*100)</f>
         <v/>
       </c>
     </row>
     <row r="170" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H170" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I170" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H171" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I171" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H172" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I172" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H173" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I173" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H174" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I174" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H175" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I175" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H176" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I176" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H177" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I177" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H178" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I178" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H179" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I179" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H180" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I180" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H181" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I181" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H182" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I182" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H183" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I183" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H184" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I184" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H185" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I185" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H186" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I186" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H187" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I187" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H188" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I188" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H189" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I189" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H190" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I190" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H191" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I191" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H192" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I192" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H193" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I193" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H194" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I194" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H195" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I195" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="196" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H196" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I196" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H197" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I197" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H198" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I198" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H199" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I199" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H200" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I200" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H201" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I201" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H202" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I202" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H203" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I203" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H204" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I204" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H205" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I205" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H206" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I206" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H207" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I207" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H208" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I208" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H209" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I209" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H210" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I210" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H211" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I211" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H212" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I212" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H213" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I213" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H214" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I214" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H215" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I215" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H216" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I216" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H217" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I217" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H218" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I218" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H219" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I219" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H220" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I220" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H221" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I221" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H222" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I222" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H223" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I223" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H224" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I224" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H225" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I225" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H226" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I226" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H227" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I227" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H228" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I228" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H229" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I229" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H230" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I230" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H231" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I231" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H232" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I232" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H233" s="12" t="str">
-        <f t="shared" ref="H233:H260" si="20">IF(OR(D233="", E233=""), "", D233-E233)</f>
+        <f t="shared" ref="H233:H260" si="22">IF(OR(D233="", E233=""), "", D233-E233)</f>
         <v/>
       </c>
       <c r="I233" s="12" t="str">
-        <f t="shared" ref="I233:I267" si="21">IF(OR(H233="",E233=0),"",ABS(H233)/E233*100)</f>
+        <f t="shared" ref="I233:I267" si="23">IF(OR(H233="",E233=0),"",ABS(H233)/E233*100)</f>
         <v/>
       </c>
     </row>
     <row r="234" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H234" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I234" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H235" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I235" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="236" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H236" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I236" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="237" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H237" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I237" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="238" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H238" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I238" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="239" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H239" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I239" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="240" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H240" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I240" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="241" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H241" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I241" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="242" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H242" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I242" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="243" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H243" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I243" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="244" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H244" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I244" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="245" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H245" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I245" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="246" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H246" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I246" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="247" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H247" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I247" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="248" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H248" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I248" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H249" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I249" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="250" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H250" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I250" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="251" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H251" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I251" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="252" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H252" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I252" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="253" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H253" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I253" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="254" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H254" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I254" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="255" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H255" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I255" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="256" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H256" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I256" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="257" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H257" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I257" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="258" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H258" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I258" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="259" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H259" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I259" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="260" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H260" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I260" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="261" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I261" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="262" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I262" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="263" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I263" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="264" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I264" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="265" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I265" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="266" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I266" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="267" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I267" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
week 6 work uploaded, week 7 planned
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BEDABE6-05EE-D84A-80D1-61245F9549CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE01DF1-DF4F-4148-869A-5E29850C1777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="171">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -634,10 +634,19 @@
     <t xml:space="preserve">Making changes to use cases, and user case description. </t>
   </si>
   <si>
-    <t xml:space="preserve">23-02-24: </t>
-  </si>
-  <si>
     <t>Week 7 (February 29 - March 6)</t>
+  </si>
+  <si>
+    <t>Implementation- Home Page</t>
+  </si>
+  <si>
+    <t>Project Plan v2</t>
+  </si>
+  <si>
+    <t>Application Running on Local Hosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-02-24: Need to make the timeline for the upcoming week, start testing cloud services. </t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I267"/>
+  <dimension ref="A1:I266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -1598,11 +1607,11 @@
       <c r="F7" s="15"/>
       <c r="G7" s="2"/>
       <c r="H7" s="12" t="str">
-        <f t="shared" ref="H7:H104" si="0">IF(OR(D7="", E7=""), "", D7-E7)</f>
+        <f t="shared" ref="H7:H103" si="0">IF(OR(D7="", E7=""), "", D7-E7)</f>
         <v/>
       </c>
       <c r="I7" s="12" t="str">
-        <f t="shared" ref="I7:I104" si="1">IF(OR(H7="",E7=0),"",ABS(H7)/E7*100)</f>
+        <f t="shared" ref="I7:I103" si="1">IF(OR(H7="",E7=0),"",ABS(H7)/E7*100)</f>
         <v/>
       </c>
     </row>
@@ -3760,16 +3769,22 @@
       <c r="D86" s="5">
         <v>5</v>
       </c>
+      <c r="E86" s="5">
+        <v>5</v>
+      </c>
+      <c r="F86" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="G86" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H86" s="12" t="str">
+        <v>170</v>
+      </c>
+      <c r="H86" s="12">
         <f>IF(OR(D86="", E86=""), "", D86-E86)</f>
-        <v/>
-      </c>
-      <c r="I86" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="I86" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.15">
@@ -3785,14 +3800,20 @@
       <c r="D87" s="5">
         <v>1</v>
       </c>
+      <c r="E87" s="5">
+        <v>1</v>
+      </c>
+      <c r="F87" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="G87" s="33"/>
-      <c r="H87" s="12" t="str">
+      <c r="H87" s="12">
         <f>IF(OR(D87="", E87=""), "", D87-E87)</f>
-        <v/>
-      </c>
-      <c r="I87" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I87" s="12">
         <f>IF(OR(H87="",E87=0),"",ABS(H87)/E87*100)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.15">
@@ -3827,6 +3848,21 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A89" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D89" s="5">
+        <v>3</v>
+      </c>
+      <c r="F89" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H89" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3837,6 +3873,21 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A90" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B90" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D90" s="5">
+        <v>5</v>
+      </c>
+      <c r="F90" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H90" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3847,6 +3898,15 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A91" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="2"/>
       <c r="H91" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3857,17 +3917,20 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A92" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="2"/>
+      <c r="A92" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="5">
+        <v>2</v>
+      </c>
       <c r="H92" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(D92="", E92=""), "", D92-E92)</f>
         <v/>
       </c>
       <c r="I92" s="12" t="str">
@@ -3876,8 +3939,20 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A93" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="5">
+        <v>2</v>
+      </c>
       <c r="H93" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(D93="", E93=""), "", D93-E93)</f>
         <v/>
       </c>
       <c r="I93" s="12" t="str">
@@ -3886,6 +3961,18 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A94" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D94" s="5">
+        <v>3</v>
+      </c>
       <c r="H94" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3896,6 +3983,18 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A95" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D95" s="5">
+        <v>4</v>
+      </c>
       <c r="H95" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3906,6 +4005,18 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A96" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D96" s="5">
+        <v>3</v>
+      </c>
       <c r="H96" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3915,7 +4026,19 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A97" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D97" s="5">
+        <v>5</v>
+      </c>
       <c r="H97" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3925,7 +4048,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H98" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3935,7 +4058,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H99" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3945,7 +4068,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H100" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3955,7 +4078,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H101" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3965,7 +4088,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H102" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3975,7 +4098,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H103" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3985,27 +4108,27 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H104" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H104:H167" si="18">IF(OR(D104="", E104=""), "", D104-E104)</f>
         <v/>
       </c>
       <c r="I104" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I104:I167" si="19">IF(OR(H104="",E104=0),"",ABS(H104)/E104*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H105" s="12" t="str">
-        <f t="shared" ref="H105:H168" si="18">IF(OR(D105="", E105=""), "", D105-E105)</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I105" s="12" t="str">
-        <f t="shared" ref="I105:I168" si="19">IF(OR(H105="",E105=0),"",ABS(H105)/E105*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H106" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4015,7 +4138,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H107" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4025,7 +4148,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H108" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4035,7 +4158,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H109" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4045,7 +4168,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H110" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4055,7 +4178,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H111" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4065,7 +4188,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H112" s="12" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -4627,21 +4750,21 @@
     </row>
     <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="H168:H231" si="20">IF(OR(D168="", E168=""), "", D168-E168)</f>
         <v/>
       </c>
       <c r="I168" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="I168:I231" si="21">IF(OR(H168="",E168=0),"",ABS(H168)/E168*100)</f>
         <v/>
       </c>
     </row>
     <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="12" t="str">
-        <f t="shared" ref="H169:H232" si="20">IF(OR(D169="", E169=""), "", D169-E169)</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I169" s="12" t="str">
-        <f t="shared" ref="I169:I232" si="21">IF(OR(H169="",E169=0),"",ABS(H169)/E169*100)</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
@@ -5267,21 +5390,21 @@
     </row>
     <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H232" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="H232:H259" si="22">IF(OR(D232="", E232=""), "", D232-E232)</f>
         <v/>
       </c>
       <c r="I232" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="I232:I266" si="23">IF(OR(H232="",E232=0),"",ABS(H232)/E232*100)</f>
         <v/>
       </c>
     </row>
     <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H233" s="12" t="str">
-        <f t="shared" ref="H233:H260" si="22">IF(OR(D233="", E233=""), "", D233-E233)</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I233" s="12" t="str">
-        <f t="shared" ref="I233:I267" si="23">IF(OR(H233="",E233=0),"",ABS(H233)/E233*100)</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
@@ -5546,10 +5669,6 @@
       </c>
     </row>
     <row r="260" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H260" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
       <c r="I260" s="12" t="str">
         <f t="shared" si="23"/>
         <v/>
@@ -5591,15 +5710,9 @@
         <v/>
       </c>
     </row>
-    <row r="267" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="I267" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="F5:F10 F12:F33 F35:F65547">
+  <conditionalFormatting sqref="F5:F10 F12:F33 F35:F65546">
     <cfRule type="cellIs" dxfId="2" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Delayed"</formula>
     </cfRule>
@@ -5611,10 +5724,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65547" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65546" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, Ongoing, Delayed, Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B58:B65547" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B98:B65546 B58:B96" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Requirements, Design, Development, Testing, Preparation, Coordination, Documentation, Interfaces, Delivery"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Week 7 completed, Week 8 scheduled
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE01DF1-DF4F-4148-869A-5E29850C1777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44D5DE9C-F549-BB48-831E-E6293943513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="183">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -647,6 +647,42 @@
   </si>
   <si>
     <t xml:space="preserve">23-02-24: Need to make the timeline for the upcoming week, start testing cloud services. </t>
+  </si>
+  <si>
+    <t>Timeline for the remaining tasks</t>
+  </si>
+  <si>
+    <t>Client meeting-15</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-15</t>
+  </si>
+  <si>
+    <t>01-03-24: Given us final reviews for design, need to start implementing, and timeline to be created on discussion with UI team</t>
+  </si>
+  <si>
+    <t>Need to make sure everyone has run the app on their local hosts, and understand the codebase for the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to discuss with UI team about their tentative plan </t>
+  </si>
+  <si>
+    <t>Final review of figma design given, implementation started for the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credentials for DigitalOcean given to us, need to run the app on the instance once. </t>
+  </si>
+  <si>
+    <t>Week 8 (March 7 - March 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Services Alternatives </t>
+  </si>
+  <si>
+    <t>Code flow testing</t>
+  </si>
+  <si>
+    <t>Testing- Home Page</t>
   </si>
 </sst>
 </file>
@@ -793,7 +829,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -897,9 +933,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1017,6 +1050,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -3421,7 +3458,7 @@
       <c r="F74" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G74" s="40" t="s">
+      <c r="G74" s="33" t="s">
         <v>160</v>
       </c>
       <c r="H74" s="12">
@@ -3450,7 +3487,7 @@
       <c r="F75" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G75" s="40" t="s">
+      <c r="G75" s="33" t="s">
         <v>151</v>
       </c>
       <c r="H75" s="12">
@@ -3506,7 +3543,7 @@
       <c r="F77" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G77" s="40" t="s">
+      <c r="G77" s="33" t="s">
         <v>158</v>
       </c>
       <c r="H77" s="12">
@@ -3537,7 +3574,7 @@
       <c r="F78" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G78" s="40" t="s">
+      <c r="G78" s="33" t="s">
         <v>152</v>
       </c>
       <c r="H78" s="12">
@@ -3597,7 +3634,7 @@
       <c r="F80" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G80" s="40" t="s">
+      <c r="G80" s="33" t="s">
         <v>159</v>
       </c>
       <c r="H80" s="12">
@@ -3685,7 +3722,7 @@
       <c r="F83" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="G83" s="40" t="s">
+      <c r="G83" s="33" t="s">
         <v>163</v>
       </c>
       <c r="H83" s="12" t="str">
@@ -3713,7 +3750,7 @@
       <c r="F84" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="G84" s="40" t="s">
+      <c r="G84" s="33" t="s">
         <v>157</v>
       </c>
       <c r="H84" s="12" t="str">
@@ -3744,7 +3781,7 @@
       <c r="F85" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G85" s="40" t="s">
+      <c r="G85" s="33" t="s">
         <v>164</v>
       </c>
       <c r="H85" s="12">
@@ -3835,7 +3872,7 @@
       <c r="F88" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G88" s="40" t="s">
+      <c r="G88" s="33" t="s">
         <v>165</v>
       </c>
       <c r="H88" s="12">
@@ -3929,13 +3966,20 @@
       <c r="D92" s="5">
         <v>2</v>
       </c>
-      <c r="H92" s="12" t="str">
+      <c r="E92" s="5">
+        <v>2</v>
+      </c>
+      <c r="F92" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G92" s="33"/>
+      <c r="H92" s="12">
         <f>IF(OR(D92="", E92=""), "", D92-E92)</f>
-        <v/>
-      </c>
-      <c r="I92" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I92" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.15">
@@ -3951,13 +3995,22 @@
       <c r="D93" s="5">
         <v>2</v>
       </c>
-      <c r="H93" s="12" t="str">
+      <c r="E93" s="5">
+        <v>1</v>
+      </c>
+      <c r="F93" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G93" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H93" s="12">
         <f>IF(OR(D93="", E93=""), "", D93-E93)</f>
-        <v/>
-      </c>
-      <c r="I93" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I93" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.15">
@@ -3973,13 +4026,20 @@
       <c r="D94" s="5">
         <v>3</v>
       </c>
-      <c r="H94" s="12" t="str">
+      <c r="E94" s="5">
+        <v>1</v>
+      </c>
+      <c r="F94" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G94" s="33"/>
+      <c r="H94" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I94" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I94" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.15">
@@ -3995,13 +4055,22 @@
       <c r="D95" s="5">
         <v>4</v>
       </c>
-      <c r="H95" s="12" t="str">
+      <c r="E95" s="5">
+        <v>1</v>
+      </c>
+      <c r="F95" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G95" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="H95" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I95" s="12" t="str">
+        <v>3</v>
+      </c>
+      <c r="I95" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>300</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.15">
@@ -4017,13 +4086,20 @@
       <c r="D96" s="5">
         <v>3</v>
       </c>
-      <c r="H96" s="12" t="str">
+      <c r="E96" s="5">
+        <v>1</v>
+      </c>
+      <c r="F96" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G96" s="33"/>
+      <c r="H96" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I96" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I96" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.15">
@@ -4039,66 +4115,176 @@
       <c r="D97" s="5">
         <v>5</v>
       </c>
-      <c r="H97" s="12" t="str">
+      <c r="E97" s="5">
+        <v>5</v>
+      </c>
+      <c r="F97" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G97" s="33"/>
+      <c r="H97" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I97" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I97" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H98" s="12" t="str">
+      <c r="A98" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D98" s="5">
+        <v>2</v>
+      </c>
+      <c r="E98" s="5">
+        <v>1</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G98" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="H98" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I98" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I98" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H99" s="12" t="str">
+      <c r="A99" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C99" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D99" s="5">
+        <v>5</v>
+      </c>
+      <c r="E99" s="5">
+        <v>5</v>
+      </c>
+      <c r="F99" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G99" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="H99" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I99" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I99" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H100" s="12" t="str">
+      <c r="A100" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" s="5">
+        <v>1</v>
+      </c>
+      <c r="E100" s="5">
+        <v>1</v>
+      </c>
+      <c r="F100" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G100" s="33"/>
+      <c r="H100" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I100" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I100" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H101" s="12" t="str">
+      <c r="A101" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C101" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="5">
+        <v>5</v>
+      </c>
+      <c r="E101" s="5">
+        <v>5</v>
+      </c>
+      <c r="F101" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G101" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="H101" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I101" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I101" s="12">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="2"/>
       <c r="H102" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H102" si="18">IF(OR(D102="", E102=""), "", D102-E102)</f>
         <v/>
       </c>
       <c r="I102" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I102" si="19">IF(OR(H102="",E102=0),"",ABS(H102)/E102*100)</f>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A103" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B103" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C103" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2</v>
+      </c>
       <c r="H103" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4109,1604 +4295,1676 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A104" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B104" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C104" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D104" s="5">
+        <v>2</v>
+      </c>
       <c r="H104" s="12" t="str">
-        <f t="shared" ref="H104:H167" si="18">IF(OR(D104="", E104=""), "", D104-E104)</f>
+        <f t="shared" ref="H104:H167" si="20">IF(OR(D104="", E104=""), "", D104-E104)</f>
         <v/>
       </c>
       <c r="I104" s="12" t="str">
-        <f t="shared" ref="I104:I167" si="19">IF(OR(H104="",E104=0),"",ABS(H104)/E104*100)</f>
+        <f t="shared" ref="I104:I167" si="21">IF(OR(H104="",E104=0),"",ABS(H104)/E104*100)</f>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A105" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C105" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D105" s="5">
+        <v>3</v>
+      </c>
       <c r="H105" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I105" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A106" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C106" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D106" s="5">
+        <v>2</v>
+      </c>
       <c r="H106" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I106" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A107" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B107" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D107" s="5">
+        <v>1</v>
+      </c>
       <c r="H107" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I107" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A108" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B108" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C108" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D108" s="5">
+        <v>5</v>
+      </c>
       <c r="H108" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I108" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A109" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C109" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D109" s="5">
+        <v>3</v>
+      </c>
       <c r="H109" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I109" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H110" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I110" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H111" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I111" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H112" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I112" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H113" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I113" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H114" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I114" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H115" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I115" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H116" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I116" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H117" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I117" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H118" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I118" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H119" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I119" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H120" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I120" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H121" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I121" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H122" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I122" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H123" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I123" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H124" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I124" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H125" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I125" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H126" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I126" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H127" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I127" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H128" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I128" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H129" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I129" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H130" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I130" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H131" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I131" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="132" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H132" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I132" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H133" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I133" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H134" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I134" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H135" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I135" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H136" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I136" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H137" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I137" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H138" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I138" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H139" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I139" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H140" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I140" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H141" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I141" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H142" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I142" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H143" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I143" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H144" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I144" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H145" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I145" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H146" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I146" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H147" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I147" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H148" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I148" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H149" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I149" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H150" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I150" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H151" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I151" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H152" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I152" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H153" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I153" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H154" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I154" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H155" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I155" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H156" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I156" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H157" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I157" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H158" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I158" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H159" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I159" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H160" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I160" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H161" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I161" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H162" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I162" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H163" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I163" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I164" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I165" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I166" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I167" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="12" t="str">
-        <f t="shared" ref="H168:H231" si="20">IF(OR(D168="", E168=""), "", D168-E168)</f>
+        <f t="shared" ref="H168:H231" si="22">IF(OR(D168="", E168=""), "", D168-E168)</f>
         <v/>
       </c>
       <c r="I168" s="12" t="str">
-        <f t="shared" ref="I168:I231" si="21">IF(OR(H168="",E168=0),"",ABS(H168)/E168*100)</f>
+        <f t="shared" ref="I168:I231" si="23">IF(OR(H168="",E168=0),"",ABS(H168)/E168*100)</f>
         <v/>
       </c>
     </row>
     <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I169" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H170" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I170" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H171" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I171" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H172" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I172" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H173" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I173" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H174" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I174" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H175" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I175" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H176" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I176" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H177" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I177" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H178" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I178" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H179" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I179" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H180" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I180" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H181" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I181" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H182" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I182" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H183" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I183" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H184" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I184" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H185" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I185" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H186" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I186" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H187" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I187" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H188" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I188" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H189" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I189" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H190" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I190" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H191" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I191" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H192" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I192" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H193" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I193" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H194" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I194" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H195" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I195" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="196" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H196" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I196" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H197" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I197" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H198" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I198" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H199" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I199" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H200" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I200" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H201" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I201" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H202" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I202" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H203" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I203" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H204" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I204" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H205" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I205" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H206" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I206" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H207" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I207" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H208" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I208" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H209" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I209" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H210" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I210" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H211" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I211" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H212" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I212" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H213" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I213" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H214" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I214" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H215" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I215" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H216" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I216" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H217" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I217" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H218" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I218" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H219" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I219" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H220" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I220" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H221" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I221" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H222" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I222" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H223" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I223" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H224" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I224" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H225" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I225" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H226" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I226" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H227" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I227" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H228" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I228" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H229" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I229" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H230" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I230" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H231" s="12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I231" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H232" s="12" t="str">
-        <f t="shared" ref="H232:H259" si="22">IF(OR(D232="", E232=""), "", D232-E232)</f>
+        <f t="shared" ref="H232:H259" si="24">IF(OR(D232="", E232=""), "", D232-E232)</f>
         <v/>
       </c>
       <c r="I232" s="12" t="str">
-        <f t="shared" ref="I232:I266" si="23">IF(OR(H232="",E232=0),"",ABS(H232)/E232*100)</f>
+        <f t="shared" ref="I232:I266" si="25">IF(OR(H232="",E232=0),"",ABS(H232)/E232*100)</f>
         <v/>
       </c>
     </row>
     <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H233" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I233" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="234" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H234" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I234" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H235" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I235" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="236" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H236" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I236" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="237" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H237" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I237" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="238" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H238" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I238" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="239" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H239" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I239" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="240" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H240" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I240" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="241" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H241" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I241" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="242" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H242" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I242" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="243" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H243" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I243" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="244" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H244" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I244" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="245" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H245" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I245" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="246" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H246" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I246" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="247" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H247" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I247" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="248" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H248" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I248" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H249" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I249" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="250" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H250" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I250" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="251" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H251" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I251" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="252" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H252" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I252" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="253" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H253" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I253" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="254" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H254" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I254" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="255" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H255" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I255" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="256" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H256" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I256" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="257" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H257" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I257" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="258" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H258" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I258" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="259" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H259" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I259" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="260" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I260" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="261" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I261" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="262" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I262" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="263" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I263" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="264" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I264" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="265" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I265" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
     <row r="266" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I266" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -5727,7 +5985,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65546" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, Ongoing, Delayed, Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B98:B65546 B58:B96" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B58:B96 B98:B65546" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Requirements, Design, Development, Testing, Preparation, Coordination, Documentation, Interfaces, Delivery"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Week 9 completed, week 10 added
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiitaphyd-my.sharepoint.com/personal/aanvik_bhatnagar_students_iiit_ac_in/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/Project_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32E10210-A312-4D1E-8A2F-4BF0735204DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C932CC3B-59D2-1E4F-B843-4FD44E1DA3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="235">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -736,29 +736,116 @@
     <t>Client meeting-18</t>
   </si>
   <si>
+    <t xml:space="preserve">08-03-24: Decision to not continue with DigitalOcean was made, asked to send a final ppt of design to be displayed to CEO. </t>
+  </si>
+  <si>
     <t>MoM Client Meet-18</t>
   </si>
   <si>
     <t>Week 9 (March 15-March 22)</t>
   </si>
   <si>
+    <t xml:space="preserve">Client has asked us to prioritize the backend development on local host, and then only focus on deploying on AWS, so it has been kept as secondary priority. </t>
+  </si>
+  <si>
     <t>Implementation- Item's Page</t>
   </si>
   <si>
+    <t>Due to high consumption of CPU by running 3-4 consecutive scans, backend server is stopping abruptly; discussed with client in meet</t>
+  </si>
+  <si>
     <t>Testing Plan v2</t>
   </si>
   <si>
+    <t>Update the use cases number according to the latest draft of SRS</t>
+  </si>
+  <si>
     <t>Backend FrameWork-Camera</t>
   </si>
   <si>
+    <t>Detection images can be viewed on item's page, errors in backend has been resolved</t>
+  </si>
+  <si>
     <t>R1 Presentation</t>
+  </si>
+  <si>
+    <t>Client meeting-19</t>
+  </si>
+  <si>
+    <t>11-03-24: Image display is still an issue that is hard to rectify, will update it on the presentation on Friday</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-19</t>
+  </si>
+  <si>
+    <t>Design Document v2</t>
+  </si>
+  <si>
+    <t>Specific naming of some classes, images also updated without grid</t>
+  </si>
+  <si>
+    <t>Client meeting-20</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Demo Video </t>
+  </si>
+  <si>
+    <t>15-03-24: First presentation of updated UI code to the client with deliverables given for R1 for client, asked to submit a demo video</t>
+  </si>
+  <si>
+    <t>Documentation Formatting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the repository, submit all the documents with a proper directory structure, and a uniform document naming format. </t>
+  </si>
+  <si>
+    <t>Chetan &amp; Rohan Sh</t>
+  </si>
+  <si>
+    <t>Testing- Camera Page</t>
+  </si>
+  <si>
+    <t>Testing- Items Page</t>
+  </si>
+  <si>
+    <t>Week 10 (March 23-March 30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Processing </t>
+  </si>
+  <si>
+    <t>Rohan N &amp; Aanvik</t>
+  </si>
+  <si>
+    <t>Aanvik &amp; Chetan</t>
+  </si>
+  <si>
+    <t>Video Viewer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 Document Update </t>
+  </si>
+  <si>
+    <t>Project synopsis v2</t>
+  </si>
+  <si>
+    <t>SRS Document v2.1</t>
+  </si>
+  <si>
+    <t>Modified some release schedules based on the updated project plan, and corrected the implementation details of camera page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified the requirements based on updates from client </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -843,11 +930,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1014,9 +1097,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1487,78 +1572,78 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="C2" s="17"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="21" customHeight="1">
+    <row r="19" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>12</v>
       </c>
@@ -1566,7 +1651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="36" customHeight="1">
+    <row r="20" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>13</v>
       </c>
@@ -1574,7 +1659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.1" customHeight="1">
+    <row r="21" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>15</v>
       </c>
@@ -1582,7 +1667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="21" customHeight="1">
+    <row r="22" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>17</v>
       </c>
@@ -1590,27 +1675,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18">
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18">
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B24" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18">
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18">
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18">
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B27" s="23"/>
     </row>
   </sheetData>
@@ -1623,26 +1708,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I266"/>
+  <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.95" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="81.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="81.5" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.95" customHeight="1">
+    <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="str">
         <f>(Instructions!A19)</f>
         <v>PROJECT NUMBER</v>
@@ -1652,7 +1737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="36.950000000000003" customHeight="1">
+    <row r="2" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="str">
         <f>(Instructions!A20)</f>
         <v>PROJECT NAME</v>
@@ -1662,7 +1747,7 @@
         <v xml:space="preserve">Computer Vision Application for Real-time Multimodal Product Detection </v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.95" customHeight="1">
+    <row r="3" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="str">
         <f>(Instructions!A21)</f>
         <v>PROJECT MENTOR (sponsor)</v>
@@ -1672,7 +1757,7 @@
         <v>Chaitanya Sagar</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="9" customFormat="1" ht="27.95">
+    <row r="5" spans="1:9" s="9" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1701,7 +1786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="19" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2">
+    <row r="6" spans="1:9" s="19" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>32</v>
       </c>
@@ -1712,7 +1797,7 @@
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" outlineLevel="2">
+    <row r="7" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1731,7 +1816,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:9" outlineLevel="2">
+    <row r="8" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1751,7 +1836,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:9" outlineLevel="2">
+    <row r="9" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1771,7 +1856,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.1" outlineLevel="2">
+    <row r="10" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
         <v>39</v>
       </c>
@@ -1796,7 +1881,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" outlineLevel="2">
+    <row r="11" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>43</v>
       </c>
@@ -1812,7 +1897,7 @@
       <c r="E11" s="5">
         <v>0.5</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="40" t="s">
         <v>41</v>
       </c>
       <c r="H11" s="12">
@@ -1823,7 +1908,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.1" customHeight="1" outlineLevel="2">
+    <row r="12" spans="1:9" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A12" s="22" t="s">
         <v>46</v>
       </c>
@@ -1854,7 +1939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.1" outlineLevel="2">
+    <row r="13" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="s">
         <v>49</v>
       </c>
@@ -1885,7 +1970,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="14" spans="1:9" outlineLevel="2">
+    <row r="14" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1910,7 +1995,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" outlineLevel="2">
+    <row r="15" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1938,7 +2023,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" outlineLevel="2">
+    <row r="16" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1969,7 +2054,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" outlineLevel="2">
+    <row r="17" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>60</v>
       </c>
@@ -2000,7 +2085,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:9" outlineLevel="2">
+    <row r="18" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
         <v>62</v>
       </c>
@@ -2028,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" outlineLevel="2">
+    <row r="19" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -2053,7 +2138,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" outlineLevel="2">
+    <row r="20" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -2070,7 +2155,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" outlineLevel="2">
+    <row r="21" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
         <v>65</v>
       </c>
@@ -2101,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" outlineLevel="2">
+    <row r="22" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
         <v>67</v>
       </c>
@@ -2129,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.1" outlineLevel="2">
+    <row r="23" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A23" s="30" t="s">
         <v>68</v>
       </c>
@@ -2160,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="27.95" outlineLevel="2">
+    <row r="24" spans="1:9" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="s">
         <v>70</v>
       </c>
@@ -2191,7 +2276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.1" outlineLevel="2">
+    <row r="25" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A25" s="30" t="s">
         <v>72</v>
       </c>
@@ -2222,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" outlineLevel="2">
+    <row r="26" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>74</v>
       </c>
@@ -2253,7 +2338,7 @@
         <v>9.0909090909090917</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="2" customFormat="1" outlineLevel="2">
+    <row r="27" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
         <v>76</v>
       </c>
@@ -2282,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.1">
+    <row r="28" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="30" t="s">
         <v>56</v>
       </c>
@@ -2310,7 +2395,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.1">
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="30" t="s">
         <v>53</v>
       </c>
@@ -2338,7 +2423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.1">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="30" t="s">
         <v>78</v>
       </c>
@@ -2360,7 +2445,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" ht="14.1">
+    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="30" t="s">
         <v>80</v>
       </c>
@@ -2388,7 +2473,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" s="2" customFormat="1" outlineLevel="2">
+    <row r="32" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
@@ -2405,7 +2490,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.1">
+    <row r="33" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="30" t="s">
         <v>56</v>
       </c>
@@ -2436,7 +2521,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14.1">
+    <row r="34" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="30" t="s">
         <v>78</v>
       </c>
@@ -2467,7 +2552,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14.1">
+    <row r="35" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="30" t="s">
         <v>80</v>
       </c>
@@ -2498,7 +2583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.1">
+    <row r="36" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="30" t="s">
         <v>86</v>
       </c>
@@ -2529,7 +2614,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.1">
+    <row r="37" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="30" t="s">
         <v>88</v>
       </c>
@@ -2560,7 +2645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.1">
+    <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="30" t="s">
         <v>90</v>
       </c>
@@ -2589,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14.1">
+    <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="30" t="s">
         <v>92</v>
       </c>
@@ -2620,7 +2705,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="14.1">
+    <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="30" t="s">
         <v>94</v>
       </c>
@@ -2651,7 +2736,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="27.95">
+    <row r="41" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="30" t="s">
         <v>96</v>
       </c>
@@ -2673,7 +2758,7 @@
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>
-    <row r="42" spans="1:9" ht="14.1">
+    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="30" t="s">
         <v>98</v>
       </c>
@@ -2695,7 +2780,7 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="1:9" ht="14.1">
+    <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="30" t="s">
         <v>101</v>
       </c>
@@ -2723,7 +2808,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>104</v>
       </c>
@@ -2742,7 +2827,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="14.1">
+    <row r="45" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="30" t="s">
         <v>105</v>
       </c>
@@ -2773,7 +2858,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="14.1">
+    <row r="46" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="30" t="s">
         <v>98</v>
       </c>
@@ -2803,7 +2888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14.1">
+    <row r="47" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="30" t="s">
         <v>101</v>
       </c>
@@ -2832,7 +2917,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14.1">
+    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="30" t="s">
         <v>109</v>
       </c>
@@ -2861,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14.1">
+    <row r="49" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="30" t="s">
         <v>111</v>
       </c>
@@ -2887,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14.1">
+    <row r="50" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="30" t="s">
         <v>112</v>
       </c>
@@ -2916,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14.1">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="30" t="s">
         <v>114</v>
       </c>
@@ -2942,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14.1">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="30" t="s">
         <v>115</v>
       </c>
@@ -2961,7 +3046,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>116</v>
       </c>
@@ -2986,7 +3071,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>117</v>
       </c>
@@ -3005,7 +3090,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14.1">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="30" t="s">
         <v>115</v>
       </c>
@@ -3036,7 +3121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -3067,7 +3152,7 @@
         <v>7.1428571428571423</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" s="32" t="s">
         <v>120</v>
       </c>
@@ -3096,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58" s="32" t="s">
         <v>122</v>
       </c>
@@ -3123,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A59" s="32" t="s">
         <v>94</v>
       </c>
@@ -3152,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A60" s="32" t="s">
         <v>124</v>
       </c>
@@ -3181,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61" s="32" t="s">
         <v>126</v>
       </c>
@@ -3210,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62" s="32" t="s">
         <v>101</v>
       </c>
@@ -3241,7 +3326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A63" s="32" t="s">
         <v>49</v>
       </c>
@@ -3270,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64" s="32" t="s">
         <v>129</v>
       </c>
@@ -3299,7 +3384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" s="32" t="s">
         <v>131</v>
       </c>
@@ -3328,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="32" t="s">
         <v>133</v>
       </c>
@@ -3348,7 +3433,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A67" s="32" t="s">
         <v>134</v>
       </c>
@@ -3377,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A68" s="32" t="s">
         <v>136</v>
       </c>
@@ -3404,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A69" s="32" t="s">
         <v>94</v>
       </c>
@@ -3433,7 +3518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A70" s="32" t="s">
         <v>138</v>
       </c>
@@ -3453,7 +3538,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="12"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A71" s="32" t="s">
         <v>140</v>
       </c>
@@ -3473,7 +3558,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A72" s="32" t="s">
         <v>142</v>
       </c>
@@ -3499,7 +3584,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>143</v>
       </c>
@@ -3518,7 +3603,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A74" s="32" t="s">
         <v>133</v>
       </c>
@@ -3547,7 +3632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75" s="32" t="s">
         <v>138</v>
       </c>
@@ -3578,7 +3663,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="32" t="s">
         <v>140</v>
       </c>
@@ -3603,7 +3688,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A77" s="32" t="s">
         <v>142</v>
       </c>
@@ -3634,7 +3719,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A78" s="32" t="s">
         <v>148</v>
       </c>
@@ -3665,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A79" s="32" t="s">
         <v>150</v>
       </c>
@@ -3694,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A80" s="32" t="s">
         <v>94</v>
       </c>
@@ -3725,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A81" s="32" t="s">
         <v>152</v>
       </c>
@@ -3756,7 +3841,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A82" s="32" t="s">
         <v>154</v>
       </c>
@@ -3785,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A83" s="32" t="s">
         <v>155</v>
       </c>
@@ -3813,7 +3898,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A84" s="32" t="s">
         <v>159</v>
       </c>
@@ -3841,7 +3926,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A85" s="32" t="s">
         <v>49</v>
       </c>
@@ -3872,7 +3957,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A86" s="32" t="s">
         <v>162</v>
       </c>
@@ -3903,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A87" s="32" t="s">
         <v>164</v>
       </c>
@@ -3932,7 +4017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A88" s="32" t="s">
         <v>165</v>
       </c>
@@ -3963,7 +4048,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A89" s="32" t="s">
         <v>167</v>
       </c>
@@ -3988,7 +4073,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="32" t="s">
         <v>168</v>
       </c>
@@ -4013,7 +4098,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>169</v>
       </c>
@@ -4032,7 +4117,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A92" s="32" t="s">
         <v>133</v>
       </c>
@@ -4061,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A93" s="32" t="s">
         <v>142</v>
       </c>
@@ -4092,7 +4177,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A94" s="32" t="s">
         <v>165</v>
       </c>
@@ -4121,7 +4206,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A95" s="32" t="s">
         <v>171</v>
       </c>
@@ -4152,7 +4237,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A96" s="32" t="s">
         <v>167</v>
       </c>
@@ -4181,7 +4266,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A97" s="32" t="s">
         <v>168</v>
       </c>
@@ -4210,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A98" s="32" t="s">
         <v>173</v>
       </c>
@@ -4241,7 +4326,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A99" s="32" t="s">
         <v>175</v>
       </c>
@@ -4272,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A100" s="32" t="s">
         <v>177</v>
       </c>
@@ -4301,7 +4386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A101" s="32" t="s">
         <v>94</v>
       </c>
@@ -4332,8 +4417,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="12.75">
-      <c r="A102" s="40" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B102" s="2"/>
@@ -4351,7 +4436,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A103" s="32" t="s">
         <v>180</v>
       </c>
@@ -4370,7 +4455,7 @@
       <c r="F103" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G103" s="29" t="s">
         <v>181</v>
       </c>
       <c r="H103" s="12">
@@ -4382,7 +4467,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A104" s="32" t="s">
         <v>165</v>
       </c>
@@ -4401,19 +4486,19 @@
       <c r="F104" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G104" s="29" t="s">
         <v>182</v>
       </c>
       <c r="H104" s="12">
-        <f t="shared" ref="H104:H166" si="20">IF(OR(D104="", E104=""), "", D104-E104)</f>
+        <f t="shared" ref="H104:H169" si="20">IF(OR(D104="", E104=""), "", D104-E104)</f>
         <v>0</v>
       </c>
       <c r="I104" s="12">
-        <f t="shared" ref="I104:I166" si="21">IF(OR(H104="",E104=0),"",ABS(H104)/E104*100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+        <f t="shared" ref="I104:I169" si="21">IF(OR(H104="",E104=0),"",ABS(H104)/E104*100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A105" s="32" t="s">
         <v>171</v>
       </c>
@@ -4432,7 +4517,7 @@
       <c r="F105" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G105" s="29" t="s">
         <v>183</v>
       </c>
       <c r="H105" s="12">
@@ -4444,7 +4529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A106" s="32" t="s">
         <v>167</v>
       </c>
@@ -4463,7 +4548,7 @@
       <c r="F106" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G106" s="29" t="s">
         <v>184</v>
       </c>
       <c r="H106" s="12">
@@ -4475,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A107" s="32" t="s">
         <v>173</v>
       </c>
@@ -4494,7 +4579,7 @@
       <c r="F107" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" s="29" t="s">
         <v>185</v>
       </c>
       <c r="H107" s="12">
@@ -4506,7 +4591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A108" s="32" t="s">
         <v>186</v>
       </c>
@@ -4525,7 +4610,7 @@
       <c r="F108" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G108" s="29" t="s">
         <v>187</v>
       </c>
       <c r="H108" s="12">
@@ -4537,7 +4622,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A109" s="32" t="s">
         <v>188</v>
       </c>
@@ -4556,6 +4641,7 @@
       <c r="F109" s="16" t="s">
         <v>51</v>
       </c>
+      <c r="G109" s="29"/>
       <c r="H109" s="12">
         <f t="shared" si="20"/>
         <v>2</v>
@@ -4565,7 +4651,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A110" s="32" t="s">
         <v>189</v>
       </c>
@@ -4584,7 +4670,7 @@
       <c r="F110" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G110" s="29" t="s">
         <v>190</v>
       </c>
       <c r="H110" s="12">
@@ -4596,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A111" s="32" t="s">
         <v>191</v>
       </c>
@@ -4615,6 +4701,7 @@
       <c r="F111" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="G111" s="29"/>
       <c r="H111" s="12">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -4624,7 +4711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A112" s="32" t="s">
         <v>192</v>
       </c>
@@ -4643,7 +4730,7 @@
       <c r="F112" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G112" s="29" t="s">
         <v>193</v>
       </c>
       <c r="H112" s="12">
@@ -4655,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A113" s="32" t="s">
         <v>194</v>
       </c>
@@ -4674,7 +4761,7 @@
       <c r="F113" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G113" s="29" t="s">
         <v>195</v>
       </c>
       <c r="H113" s="12">
@@ -4686,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A114" s="32" t="s">
         <v>196</v>
       </c>
@@ -4705,6 +4792,7 @@
       <c r="F114" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="G114" s="29"/>
       <c r="H114" s="12">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -4714,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A115" s="32" t="s">
         <v>197</v>
       </c>
@@ -4733,6 +4821,7 @@
       <c r="F115" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="G115" s="29"/>
       <c r="H115" s="12">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -4742,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A116" s="32" t="s">
         <v>199</v>
       </c>
@@ -4761,6 +4850,9 @@
       <c r="F116" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="G116" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="H116" s="12">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -4770,9 +4862,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A117" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B117" t="s">
         <v>44</v>
@@ -4789,6 +4881,7 @@
       <c r="F117" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="G117" s="29"/>
       <c r="H117" s="12">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -4798,9 +4891,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="12.75">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A118" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B118" s="36"/>
       <c r="C118" s="37"/>
@@ -4817,7 +4910,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>180</v>
       </c>
@@ -4831,7 +4924,10 @@
         <v>2</v>
       </c>
       <c r="F119" s="16" t="s">
-        <v>51</v>
+        <v>157</v>
+      </c>
+      <c r="G119" s="29" t="s">
+        <v>203</v>
       </c>
       <c r="H119" s="12" t="str">
         <f t="shared" si="20"/>
@@ -4842,9 +4938,9 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B120" t="s">
         <v>156</v>
@@ -4855,19 +4951,23 @@
       <c r="D120" s="5">
         <v>4</v>
       </c>
+      <c r="E120" s="5">
+        <v>4.5</v>
+      </c>
       <c r="F120" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H120" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="G120" s="29"/>
+      <c r="H120" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I120" s="12" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="I120" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v>11.111111111111111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>188</v>
       </c>
@@ -4880,21 +4980,27 @@
       <c r="D121" s="5">
         <v>3</v>
       </c>
+      <c r="E121" s="5">
+        <v>3</v>
+      </c>
       <c r="F121" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H121" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="G121" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="H121" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I121" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I121" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B122" t="s">
         <v>44</v>
@@ -4905,149 +5011,345 @@
       <c r="D122" s="5">
         <v>2</v>
       </c>
+      <c r="E122" s="5">
+        <v>2</v>
+      </c>
       <c r="F122" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H122" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="G122" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H122" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I122" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I122" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B123" t="s">
         <v>156</v>
       </c>
-      <c r="C123" s="5" t="s">
-        <v>40</v>
+      <c r="C123" s="31" t="s">
+        <v>228</v>
       </c>
       <c r="D123" s="5">
         <v>3</v>
       </c>
+      <c r="E123" s="5">
+        <v>5</v>
+      </c>
       <c r="F123" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H123" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="G123" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H123" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I123" s="12" t="str">
+        <v>-2</v>
+      </c>
+      <c r="I123" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B124" t="s">
         <v>44</v>
       </c>
-      <c r="C124" s="5" t="s">
+      <c r="C124" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D124" s="5">
+        <v>3</v>
+      </c>
+      <c r="E124" s="5">
+        <v>3</v>
+      </c>
+      <c r="F124" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G124" s="29"/>
+      <c r="H124" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I124" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A125" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B125" t="s">
+        <v>35</v>
+      </c>
+      <c r="C125" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D125" s="5">
+        <v>5</v>
+      </c>
+      <c r="E125" s="5">
+        <v>5</v>
+      </c>
+      <c r="F125" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G125" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="H125" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I125" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A126" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B126" t="s">
+        <v>44</v>
+      </c>
+      <c r="C126" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D126" s="5">
+        <v>1</v>
+      </c>
+      <c r="E126" s="5">
+        <v>1</v>
+      </c>
+      <c r="F126" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G126" s="29"/>
+      <c r="H126" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I126" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A127" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="B127" t="s">
+        <v>44</v>
+      </c>
+      <c r="C127" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D124" s="5">
+      <c r="D127" s="5">
+        <v>1</v>
+      </c>
+      <c r="E127" s="5">
+        <v>1</v>
+      </c>
+      <c r="F127" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G127" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="H127" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I127" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A128" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="B128" t="s">
+        <v>35</v>
+      </c>
+      <c r="C128" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D128" s="5">
+        <v>5</v>
+      </c>
+      <c r="E128" s="5">
+        <v>5</v>
+      </c>
+      <c r="F128" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G128" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="H128" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I128" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A129" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B129" t="s">
+        <v>44</v>
+      </c>
+      <c r="C129" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D129" s="5">
+        <v>1</v>
+      </c>
+      <c r="E129" s="5">
+        <v>1</v>
+      </c>
+      <c r="F129" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G129" s="29"/>
+      <c r="H129" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I129" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A130" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B130" t="s">
+        <v>44</v>
+      </c>
+      <c r="C130" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D130" s="5">
+        <v>1</v>
+      </c>
+      <c r="E130" s="5">
+        <v>1</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G130" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="H130" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I130" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A131" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="B131" t="s">
+        <v>44</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D131" s="5">
+        <v>1</v>
+      </c>
+      <c r="E131" s="5">
+        <v>1</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G131" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="H131" s="12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I131" s="12">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A132" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B132" t="s">
+        <v>141</v>
+      </c>
+      <c r="C132" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D132" s="5">
         <v>2</v>
       </c>
-      <c r="F124" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H124" s="12" t="str">
+      <c r="E132" s="5">
+        <v>2</v>
+      </c>
+      <c r="F132" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G132" s="29"/>
+      <c r="H132" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I124" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I132" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
-      <c r="H125" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I125" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
-      <c r="H126" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I126" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
-      <c r="H127" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I127" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
-      <c r="H128" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I128" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="129" spans="8:9">
-      <c r="H129" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I129" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="130" spans="8:9">
-      <c r="H130" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I130" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="131" spans="8:9">
-      <c r="H131" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I131" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="132" spans="8:9">
-      <c r="H132" s="12" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I132" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="133" spans="8:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A133" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B133" t="s">
+        <v>44</v>
+      </c>
+      <c r="C133" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D133" s="5">
+        <v>2</v>
+      </c>
+      <c r="F133" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G133" s="35" t="s">
+        <v>221</v>
+      </c>
       <c r="H133" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5057,7 +5359,22 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="8:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A134" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B134" t="s">
+        <v>156</v>
+      </c>
+      <c r="C134" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D134" s="5">
+        <v>5</v>
+      </c>
+      <c r="F134" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H134" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5067,7 +5384,22 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="8:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A135" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B135" t="s">
+        <v>156</v>
+      </c>
+      <c r="C135" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135" s="5">
+        <v>5</v>
+      </c>
+      <c r="F135" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H135" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5077,7 +5409,22 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="8:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A136" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B136" t="s">
+        <v>141</v>
+      </c>
+      <c r="C136" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D136" s="5">
+        <v>3</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H136" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5087,7 +5434,22 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="8:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A137" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B137" t="s">
+        <v>44</v>
+      </c>
+      <c r="C137" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="D137" s="5">
+        <v>3</v>
+      </c>
+      <c r="F137" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H137" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5097,7 +5459,22 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="8:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A138" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B138" t="s">
+        <v>141</v>
+      </c>
+      <c r="C138" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D138" s="5">
+        <v>3</v>
+      </c>
+      <c r="F138" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H138" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5107,7 +5484,16 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="8:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A139" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="B139" s="36"/>
+      <c r="C139" s="37"/>
+      <c r="D139" s="37"/>
+      <c r="E139" s="37"/>
+      <c r="F139" s="38"/>
+      <c r="G139" s="36"/>
       <c r="H139" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5117,7 +5503,19 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="8:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A140" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B140" t="s">
+        <v>44</v>
+      </c>
+      <c r="C140" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D140" s="5">
+        <v>2</v>
+      </c>
       <c r="H140" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5127,7 +5525,19 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="8:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A141" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B141" t="s">
+        <v>156</v>
+      </c>
+      <c r="C141" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D141" s="5">
+        <v>5</v>
+      </c>
       <c r="H141" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5137,7 +5547,19 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="8:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A142" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B142" t="s">
+        <v>156</v>
+      </c>
+      <c r="C142" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D142" s="5">
+        <v>5</v>
+      </c>
       <c r="H142" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5147,7 +5569,19 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="8:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A143" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B143" t="s">
+        <v>141</v>
+      </c>
+      <c r="C143" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D143" s="5">
+        <v>3</v>
+      </c>
       <c r="H143" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5157,7 +5591,19 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="8:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A144" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B144" t="s">
+        <v>141</v>
+      </c>
+      <c r="C144" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D144" s="5">
+        <v>3</v>
+      </c>
       <c r="H144" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5167,7 +5613,19 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="8:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A145" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B145" t="s">
+        <v>44</v>
+      </c>
+      <c r="C145" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="D145" s="5">
+        <v>3</v>
+      </c>
       <c r="H145" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5177,7 +5635,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="8:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H146" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5187,7 +5645,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="8:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H147" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5197,7 +5655,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="8:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H148" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5207,7 +5665,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="8:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H149" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5217,7 +5675,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="8:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H150" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5227,7 +5685,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="8:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H151" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5237,7 +5695,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="8:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H152" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5247,7 +5705,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="8:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H153" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5257,7 +5715,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="8:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H154" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5267,7 +5725,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="8:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H155" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5277,7 +5735,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="8:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H156" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5287,7 +5745,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="8:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H157" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5297,7 +5755,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="8:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H158" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5307,7 +5765,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="8:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H159" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5317,7 +5775,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="8:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H160" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5327,7 +5785,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="8:9">
+    <row r="161" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H161" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5337,7 +5795,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="8:9">
+    <row r="162" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H162" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5347,7 +5805,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="8:9">
+    <row r="163" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H163" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5357,7 +5815,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="8:9">
+    <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5367,7 +5825,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="8:9">
+    <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5377,7 +5835,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="8:9">
+    <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5387,47 +5845,47 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="8:9">
+    <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="12" t="str">
-        <f t="shared" ref="H167:H230" si="22">IF(OR(D167="", E167=""), "", D167-E167)</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I167" s="12" t="str">
-        <f t="shared" ref="I167:I230" si="23">IF(OR(H167="",E167=0),"",ABS(H167)/E167*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="168" spans="8:9">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I168" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="169" spans="8:9">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I169" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="170" spans="8:9">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H170" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="H170:H233" si="22">IF(OR(D170="", E170=""), "", D170-E170)</f>
         <v/>
       </c>
       <c r="I170" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="171" spans="8:9">
+        <f t="shared" ref="I170:I233" si="23">IF(OR(H170="",E170=0),"",ABS(H170)/E170*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H171" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5437,7 +5895,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="8:9">
+    <row r="172" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H172" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5447,7 +5905,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="8:9">
+    <row r="173" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H173" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5457,7 +5915,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="8:9">
+    <row r="174" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H174" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5467,7 +5925,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="8:9">
+    <row r="175" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H175" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5477,7 +5935,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="8:9">
+    <row r="176" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H176" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5487,7 +5945,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="8:9">
+    <row r="177" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H177" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5497,7 +5955,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="8:9">
+    <row r="178" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H178" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5507,7 +5965,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="8:9">
+    <row r="179" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H179" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5517,7 +5975,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="8:9">
+    <row r="180" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H180" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5527,7 +5985,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="8:9">
+    <row r="181" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H181" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5537,7 +5995,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="8:9">
+    <row r="182" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H182" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5547,7 +6005,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="8:9">
+    <row r="183" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H183" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5557,7 +6015,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="8:9">
+    <row r="184" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H184" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5567,7 +6025,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="8:9">
+    <row r="185" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H185" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5577,7 +6035,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="8:9">
+    <row r="186" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H186" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5587,7 +6045,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="8:9">
+    <row r="187" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H187" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5597,7 +6055,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="8:9">
+    <row r="188" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H188" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5607,7 +6065,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="8:9">
+    <row r="189" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H189" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5617,7 +6075,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="8:9">
+    <row r="190" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H190" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5627,7 +6085,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="8:9">
+    <row r="191" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H191" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5637,7 +6095,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="8:9">
+    <row r="192" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H192" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5647,7 +6105,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="8:9">
+    <row r="193" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H193" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5657,7 +6115,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="8:9">
+    <row r="194" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H194" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5667,7 +6125,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="8:9">
+    <row r="195" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H195" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5677,7 +6135,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="8:9">
+    <row r="196" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H196" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5687,7 +6145,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="8:9">
+    <row r="197" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H197" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5697,7 +6155,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="8:9">
+    <row r="198" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H198" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5707,7 +6165,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="8:9">
+    <row r="199" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H199" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5717,7 +6175,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="8:9">
+    <row r="200" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H200" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5727,7 +6185,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="8:9">
+    <row r="201" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H201" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5737,7 +6195,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="8:9">
+    <row r="202" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H202" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5747,7 +6205,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="8:9">
+    <row r="203" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H203" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5757,7 +6215,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="8:9">
+    <row r="204" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H204" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5767,7 +6225,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="8:9">
+    <row r="205" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H205" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5777,7 +6235,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="8:9">
+    <row r="206" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H206" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5787,7 +6245,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="8:9">
+    <row r="207" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H207" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5797,7 +6255,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="8:9">
+    <row r="208" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H208" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5807,7 +6265,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="8:9">
+    <row r="209" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H209" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5817,7 +6275,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="8:9">
+    <row r="210" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H210" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5827,7 +6285,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="8:9">
+    <row r="211" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H211" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5837,7 +6295,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="8:9">
+    <row r="212" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H212" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5847,7 +6305,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="8:9">
+    <row r="213" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H213" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5857,7 +6315,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="8:9">
+    <row r="214" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H214" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5867,7 +6325,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="8:9">
+    <row r="215" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H215" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5877,7 +6335,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="8:9">
+    <row r="216" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H216" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5887,7 +6345,7 @@
         <v/>
       </c>
     </row>
-    <row r="217" spans="8:9">
+    <row r="217" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H217" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5897,7 +6355,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="8:9">
+    <row r="218" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H218" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5907,7 +6365,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="8:9">
+    <row r="219" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H219" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5917,7 +6375,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="8:9">
+    <row r="220" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H220" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5927,7 +6385,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="8:9">
+    <row r="221" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H221" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5937,7 +6395,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="8:9">
+    <row r="222" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H222" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5947,7 +6405,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="8:9">
+    <row r="223" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H223" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5957,7 +6415,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="8:9">
+    <row r="224" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H224" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5967,7 +6425,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="8:9">
+    <row r="225" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H225" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5977,7 +6435,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="8:9">
+    <row r="226" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H226" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5987,7 +6445,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="8:9">
+    <row r="227" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H227" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5997,7 +6455,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="8:9">
+    <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H228" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6007,7 +6465,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="8:9">
+    <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H229" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6017,7 +6475,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="8:9">
+    <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H230" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6027,47 +6485,47 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="8:9">
+    <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H231" s="12" t="str">
-        <f t="shared" ref="H231:H258" si="24">IF(OR(D231="", E231=""), "", D231-E231)</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I231" s="12" t="str">
-        <f t="shared" ref="I231:I265" si="25">IF(OR(H231="",E231=0),"",ABS(H231)/E231*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="232" spans="8:9">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+    </row>
+    <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H232" s="12" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I232" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-    </row>
-    <row r="233" spans="8:9">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+    </row>
+    <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H233" s="12" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I233" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-    </row>
-    <row r="234" spans="8:9">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+    </row>
+    <row r="234" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H234" s="12" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="H234:H261" si="24">IF(OR(D234="", E234=""), "", D234-E234)</f>
         <v/>
       </c>
       <c r="I234" s="12" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-    </row>
-    <row r="235" spans="8:9">
+        <f t="shared" ref="I234:I268" si="25">IF(OR(H234="",E234=0),"",ABS(H234)/E234*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="235" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H235" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6077,7 +6535,7 @@
         <v/>
       </c>
     </row>
-    <row r="236" spans="8:9">
+    <row r="236" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H236" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6087,7 +6545,7 @@
         <v/>
       </c>
     </row>
-    <row r="237" spans="8:9">
+    <row r="237" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H237" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6097,7 +6555,7 @@
         <v/>
       </c>
     </row>
-    <row r="238" spans="8:9">
+    <row r="238" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H238" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6107,7 +6565,7 @@
         <v/>
       </c>
     </row>
-    <row r="239" spans="8:9">
+    <row r="239" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H239" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6117,7 +6575,7 @@
         <v/>
       </c>
     </row>
-    <row r="240" spans="8:9">
+    <row r="240" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H240" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6127,7 +6585,7 @@
         <v/>
       </c>
     </row>
-    <row r="241" spans="8:9">
+    <row r="241" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H241" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6137,7 +6595,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="8:9">
+    <row r="242" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H242" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6147,7 +6605,7 @@
         <v/>
       </c>
     </row>
-    <row r="243" spans="8:9">
+    <row r="243" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H243" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6157,7 +6615,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="8:9">
+    <row r="244" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H244" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6167,7 +6625,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="8:9">
+    <row r="245" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H245" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6177,7 +6635,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="8:9">
+    <row r="246" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H246" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6187,7 +6645,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="8:9">
+    <row r="247" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H247" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6197,7 +6655,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="8:9">
+    <row r="248" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H248" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6207,7 +6665,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="8:9">
+    <row r="249" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H249" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6217,7 +6675,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="8:9">
+    <row r="250" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H250" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6227,7 +6685,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="8:9">
+    <row r="251" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H251" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6237,7 +6695,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="8:9">
+    <row r="252" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H252" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6247,7 +6705,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="8:9">
+    <row r="253" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H253" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6257,7 +6715,7 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="8:9">
+    <row r="254" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H254" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6267,7 +6725,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="8:9">
+    <row r="255" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H255" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6277,7 +6735,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="8:9">
+    <row r="256" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H256" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6287,7 +6745,7 @@
         <v/>
       </c>
     </row>
-    <row r="257" spans="8:9">
+    <row r="257" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H257" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6297,7 +6755,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="8:9">
+    <row r="258" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H258" s="12" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -6307,52 +6765,81 @@
         <v/>
       </c>
     </row>
-    <row r="259" spans="8:9">
+    <row r="259" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H259" s="12" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
       <c r="I259" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="260" spans="8:9">
+    <row r="260" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H260" s="12" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
       <c r="I260" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="261" spans="8:9">
+    <row r="261" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H261" s="12" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
       <c r="I261" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="262" spans="8:9">
+    <row r="262" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I262" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="263" spans="8:9">
+    <row r="263" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I263" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="264" spans="8:9">
+    <row r="264" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I264" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="265" spans="8:9">
+    <row r="265" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I265" s="12" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
-    <row r="266" spans="8:9" ht="12.75"/>
+    <row r="266" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I266" s="12" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+    </row>
+    <row r="267" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I267" s="12" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+    </row>
+    <row r="268" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="I268" s="12" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="F5:F10 F12:F33 F35:F65545">
+  <conditionalFormatting sqref="F5:F10 F12:F33 F35:F65548">
     <cfRule type="cellIs" dxfId="2" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Delayed"</formula>
     </cfRule>
@@ -6364,10 +6851,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65545" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10 F12:F33 F35:F65548" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, Ongoing, Delayed, Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B58:B96 B98:B65545" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B10 B12:B33 B35:B56 B58:B96 B98:B65548" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Requirements, Design, Development, Testing, Preparation, Coordination, Documentation, Interfaces, Delivery"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Week 10 updated, and ongoing, Week 11 planned
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/Project_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C932CC3B-59D2-1E4F-B843-4FD44E1DA3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4625BAFB-6CF6-394D-8D86-4F83342B4DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="253">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -839,6 +839,60 @@
   </si>
   <si>
     <t xml:space="preserve">Modified the requirements based on updates from client </t>
+  </si>
+  <si>
+    <t>Client meeting-21</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18-03-24: Meet with the CEO, gave full demo for image and video capture. Mentioned changes in alignment, and a more real time video processing </t>
+  </si>
+  <si>
+    <t>Client meeting-22</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-22</t>
+  </si>
+  <si>
+    <t>Client meeting-23</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22-03-24: Updated the UI, need to update the PPT with the changes that CEO mentioned again from the recording, shifted Rohan S to backend team. </t>
+  </si>
+  <si>
+    <t>20-03-24: AWS credentials will be sent, need to provide a new timeline for the remaining tasks, look into replacing the file structure for a new ML Algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figuring out how to process videos on a more real time basis </t>
+  </si>
+  <si>
+    <t>Figuring out how to view video frames in detected images page</t>
+  </si>
+  <si>
+    <t>Cloud Service Alternative</t>
+  </si>
+  <si>
+    <t>AWS Instance creation and run</t>
+  </si>
+  <si>
+    <t>Modularity of Codebase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the code modular for any CV algorithm </t>
+  </si>
+  <si>
+    <t>Integration Testing</t>
+  </si>
+  <si>
+    <t>Rohan N &amp; Rohan Sh</t>
+  </si>
+  <si>
+    <t>Week 11 (March 31-April 6)</t>
   </si>
 </sst>
 </file>
@@ -1710,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -5259,7 +5313,7 @@
       <c r="F130" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G130" s="41" t="s">
+      <c r="G130" s="29" t="s">
         <v>234</v>
       </c>
       <c r="H130" s="12">
@@ -5516,13 +5570,20 @@
       <c r="D140" s="5">
         <v>2</v>
       </c>
-      <c r="H140" s="12" t="str">
+      <c r="E140" s="5">
+        <v>2</v>
+      </c>
+      <c r="F140" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G140" s="29"/>
+      <c r="H140" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I140" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I140" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.15">
@@ -5538,13 +5599,22 @@
       <c r="D141" s="5">
         <v>5</v>
       </c>
-      <c r="H141" s="12" t="str">
+      <c r="E141" s="5">
+        <v>3</v>
+      </c>
+      <c r="F141" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G141" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="H141" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I141" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I141" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.15">
@@ -5560,13 +5630,22 @@
       <c r="D142" s="5">
         <v>5</v>
       </c>
-      <c r="H142" s="12" t="str">
+      <c r="E142" s="5">
+        <v>3</v>
+      </c>
+      <c r="F142" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G142" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="H142" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I142" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I142" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.15">
@@ -5582,13 +5661,20 @@
       <c r="D143" s="5">
         <v>3</v>
       </c>
-      <c r="H143" s="12" t="str">
+      <c r="E143" s="5">
+        <v>3</v>
+      </c>
+      <c r="F143" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G143" s="29"/>
+      <c r="H143" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I143" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I143" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.15">
@@ -5604,13 +5690,20 @@
       <c r="D144" s="5">
         <v>3</v>
       </c>
-      <c r="H144" s="12" t="str">
+      <c r="E144" s="5">
+        <v>2</v>
+      </c>
+      <c r="F144" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G144" s="29"/>
+      <c r="H144" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I144" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I144" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>50</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.15">
@@ -5626,76 +5719,220 @@
       <c r="D145" s="5">
         <v>3</v>
       </c>
-      <c r="H145" s="12" t="str">
+      <c r="E145" s="5">
+        <v>3</v>
+      </c>
+      <c r="F145" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G145" s="29"/>
+      <c r="H145" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I145" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I145" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H146" s="12" t="str">
+      <c r="A146" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B146" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D146" s="5">
+        <v>5</v>
+      </c>
+      <c r="E146" s="5">
+        <v>5</v>
+      </c>
+      <c r="F146" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G146" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="H146" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I146" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I146" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H147" s="12" t="str">
+      <c r="A147" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B147" t="s">
+        <v>44</v>
+      </c>
+      <c r="C147" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D147" s="5">
+        <v>1</v>
+      </c>
+      <c r="E147" s="5">
+        <v>1</v>
+      </c>
+      <c r="F147" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G147" s="29"/>
+      <c r="H147" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I147" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I147" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H148" s="12" t="str">
+      <c r="A148" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B148" t="s">
+        <v>35</v>
+      </c>
+      <c r="C148" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D148" s="5">
+        <v>5</v>
+      </c>
+      <c r="E148" s="5">
+        <v>5</v>
+      </c>
+      <c r="F148" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G148" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="H148" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I148" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I148" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H149" s="12" t="str">
+      <c r="A149" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B149" t="s">
+        <v>44</v>
+      </c>
+      <c r="C149" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D149" s="5">
+        <v>1</v>
+      </c>
+      <c r="E149" s="5">
+        <v>1</v>
+      </c>
+      <c r="F149" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G149" s="29"/>
+      <c r="H149" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I149" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I149" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H150" s="12" t="str">
+      <c r="A150" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B150" t="s">
+        <v>35</v>
+      </c>
+      <c r="C150" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D150" s="5">
+        <v>5</v>
+      </c>
+      <c r="E150" s="5">
+        <v>5</v>
+      </c>
+      <c r="F150" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G150" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="H150" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I150" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I150" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H151" s="12" t="str">
+      <c r="A151" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B151" t="s">
+        <v>44</v>
+      </c>
+      <c r="C151" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D151" s="5">
+        <v>1</v>
+      </c>
+      <c r="E151" s="5">
+        <v>1</v>
+      </c>
+      <c r="F151" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H151" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I151" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I151" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A152" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B152" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D152" s="5">
+        <v>5</v>
+      </c>
+      <c r="F152" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G152" s="41" t="s">
+        <v>247</v>
+      </c>
       <c r="H152" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5706,6 +5943,24 @@
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A153" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B153" t="s">
+        <v>156</v>
+      </c>
+      <c r="C153" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D153" s="5">
+        <v>6</v>
+      </c>
+      <c r="F153" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G153" s="41" t="s">
+        <v>249</v>
+      </c>
       <c r="H153" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5716,6 +5971,21 @@
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A154" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B154" t="s">
+        <v>141</v>
+      </c>
+      <c r="C154" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="D154" s="5">
+        <v>4</v>
+      </c>
+      <c r="F154" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H154" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -5726,6 +5996,15 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A155" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="B155" s="36"/>
+      <c r="C155" s="37"/>
+      <c r="D155" s="37"/>
+      <c r="E155" s="37"/>
+      <c r="F155" s="38"/>
+      <c r="G155" s="36"/>
       <c r="H155" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>

</xml_diff>

<commit_message>
Week 11 completed, Week 12 planned
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/Project_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4625BAFB-6CF6-394D-8D86-4F83342B4DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3E3AECD-6664-3546-8D8A-A887C7691713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="264">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -893,6 +893,39 @@
   </si>
   <si>
     <t>Week 11 (March 31-April 6)</t>
+  </si>
+  <si>
+    <t>Client meeting-24</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27-03-24: Discussed that we will need more time to implement the real time video part, asked UI team to make some minor changes in alignment and colour. </t>
+  </si>
+  <si>
+    <t>Shifting the complete team to backend, and planning work after Quiz 2</t>
+  </si>
+  <si>
+    <t>Refactoring the code to try and display the image frames, and need to store them somewhere, and then process them on the frontend</t>
+  </si>
+  <si>
+    <t>Video runs on a loop when played, pauses when clicked pause on the video player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS layout understood, read how to create an instance and operate on it </t>
+  </si>
+  <si>
+    <t>R1 Code Evaluation</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Looking into how to replace the CV algorithm</t>
+  </si>
+  <si>
+    <t>Week 12 (April 7-April 14)</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1080,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1153,9 +1186,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1764,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -5754,7 +5784,7 @@
       <c r="F146" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G146" s="41" t="s">
+      <c r="G146" s="29" t="s">
         <v>237</v>
       </c>
       <c r="H146" s="12">
@@ -5930,7 +5960,7 @@
       <c r="F152" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G152" s="41" t="s">
+      <c r="G152" s="29" t="s">
         <v>247</v>
       </c>
       <c r="H152" s="12" t="str">
@@ -5958,7 +5988,7 @@
       <c r="F153" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G153" s="41" t="s">
+      <c r="G153" s="29" t="s">
         <v>249</v>
       </c>
       <c r="H153" s="12" t="str">
@@ -6015,96 +6045,292 @@
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H156" s="12" t="str">
+      <c r="A156" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B156" t="s">
+        <v>156</v>
+      </c>
+      <c r="C156" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D156" s="5">
+        <v>2</v>
+      </c>
+      <c r="E156" s="5">
+        <v>2</v>
+      </c>
+      <c r="F156" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G156" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="H156" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I156" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I156" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H157" s="12" t="str">
+      <c r="A157" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B157" t="s">
+        <v>156</v>
+      </c>
+      <c r="C157" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D157" s="5">
+        <v>2</v>
+      </c>
+      <c r="E157" s="5">
+        <v>2</v>
+      </c>
+      <c r="F157" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G157" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="H157" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I157" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I157" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H158" s="12" t="str">
+      <c r="A158" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B158" t="s">
+        <v>141</v>
+      </c>
+      <c r="C158" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D158" s="5">
+        <v>1</v>
+      </c>
+      <c r="E158" s="5">
+        <v>1</v>
+      </c>
+      <c r="F158" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G158" s="29"/>
+      <c r="H158" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I158" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I158" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H159" s="12" t="str">
+      <c r="A159" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B159" t="s">
+        <v>38</v>
+      </c>
+      <c r="C159" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D159" s="5">
+        <v>5</v>
+      </c>
+      <c r="E159" s="5">
+        <v>3</v>
+      </c>
+      <c r="F159" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G159" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="H159" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I159" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I159" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H160" s="12" t="str">
+      <c r="A160" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B160" t="s">
+        <v>156</v>
+      </c>
+      <c r="C160" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D160" s="5">
+        <v>6</v>
+      </c>
+      <c r="E160" s="5">
+        <v>4</v>
+      </c>
+      <c r="F160" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G160" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="H160" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I160" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I160" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="161" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H161" s="12" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A161" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B161" t="s">
+        <v>141</v>
+      </c>
+      <c r="C161" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="D161" s="5">
+        <v>4</v>
+      </c>
+      <c r="E161" s="5">
+        <v>3</v>
+      </c>
+      <c r="F161" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G161" s="29"/>
+      <c r="H161" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I161" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I161" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="162" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H162" s="12" t="str">
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A162" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B162" t="s">
+        <v>35</v>
+      </c>
+      <c r="C162" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D162" s="5">
+        <v>5</v>
+      </c>
+      <c r="E162" s="5">
+        <v>5</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G162" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="H162" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I162" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I162" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="163" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H163" s="12" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A163" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="B163" t="s">
+        <v>44</v>
+      </c>
+      <c r="C163" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D163" s="5">
+        <v>1</v>
+      </c>
+      <c r="E163" s="5">
+        <v>1</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G163" s="29"/>
+      <c r="H163" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I163" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I163" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="164" spans="8:9" x14ac:dyDescent="0.15">
-      <c r="H164" s="12" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A164" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B164" t="s">
+        <v>35</v>
+      </c>
+      <c r="C164" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D164" s="5">
+        <v>5</v>
+      </c>
+      <c r="E164" s="5">
+        <v>5</v>
+      </c>
+      <c r="F164" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G164" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="H164" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I164" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I164" s="12">
         <f t="shared" si="21"/>
-        <v/>
-      </c>
-    </row>
-    <row r="165" spans="8:9" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A165" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="B165" t="s">
+        <v>261</v>
+      </c>
+      <c r="C165" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F165" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G165" s="29"/>
       <c r="H165" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -6114,7 +6340,16 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A166" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="B166" s="36"/>
+      <c r="C166" s="37"/>
+      <c r="D166" s="37"/>
+      <c r="E166" s="37"/>
+      <c r="F166" s="38"/>
+      <c r="G166" s="36"/>
       <c r="H166" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -6124,7 +6359,22 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A167" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B167" t="s">
+        <v>156</v>
+      </c>
+      <c r="C167" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D167" s="5">
+        <v>4</v>
+      </c>
+      <c r="F167" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H167" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -6134,7 +6384,22 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A168" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B168" t="s">
+        <v>156</v>
+      </c>
+      <c r="C168" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D168" s="5">
+        <v>3</v>
+      </c>
+      <c r="F168" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H168" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -6144,7 +6409,22 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A169" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B169" t="s">
+        <v>141</v>
+      </c>
+      <c r="C169" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="D169" s="5">
+        <v>2</v>
+      </c>
+      <c r="F169" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H169" s="12" t="str">
         <f t="shared" si="20"/>
         <v/>
@@ -6154,7 +6434,22 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A170" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B170" t="s">
+        <v>156</v>
+      </c>
+      <c r="C170" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D170" s="5">
+        <v>3</v>
+      </c>
+      <c r="F170" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H170" s="12" t="str">
         <f t="shared" ref="H170:H233" si="22">IF(OR(D170="", E170=""), "", D170-E170)</f>
         <v/>
@@ -6164,7 +6459,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H171" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6174,7 +6469,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H172" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6184,7 +6479,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H173" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6194,7 +6489,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H174" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6204,7 +6499,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H175" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6214,7 +6509,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H176" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>

</xml_diff>

<commit_message>
Week 12 Completed, Week 13 Planned
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/Project_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3E3AECD-6664-3546-8D8A-A887C7691713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{471C2595-73D6-5B4F-B180-2232A1947209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="274">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -926,6 +926,36 @@
   </si>
   <si>
     <t>Week 12 (April 7-April 14)</t>
+  </si>
+  <si>
+    <t>Client meeting-25</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-25</t>
+  </si>
+  <si>
+    <t>AWS Deployment Run</t>
+  </si>
+  <si>
+    <t>Video Processing Part 2</t>
+  </si>
+  <si>
+    <t>Test Plan Tracker Update</t>
+  </si>
+  <si>
+    <t>Integration: Video and Items Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05-04-24: After quiz 2 we updated the client regarding progress with AWS and video processing, need to provide a plan before the final presentation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS On-Demand instance is chosen for testing existing code base. Credentials for the same given, and also ran an instance. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to start taking photos asynchronously and processing the video frame by frame. Hence, need to re-evalulate the whole video processing part. </t>
+  </si>
+  <si>
+    <t>Week 13 (April 15-April 22)</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1110,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1186,6 +1216,10 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1794,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="B178" sqref="B178"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -6372,16 +6406,22 @@
       <c r="D167" s="5">
         <v>4</v>
       </c>
+      <c r="E167" s="5">
+        <v>4</v>
+      </c>
       <c r="F167" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H167" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="G167" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="H167" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I167" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I167" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.15">
@@ -6397,16 +6437,19 @@
       <c r="D168" s="5">
         <v>3</v>
       </c>
+      <c r="E168" s="5">
+        <v>3</v>
+      </c>
       <c r="F168" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H168" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="H168" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I168" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I168" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.15">
@@ -6422,16 +6465,19 @@
       <c r="D169" s="5">
         <v>2</v>
       </c>
+      <c r="E169" s="5">
+        <v>2</v>
+      </c>
       <c r="F169" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H169" s="12" t="str">
+        <v>41</v>
+      </c>
+      <c r="H169" s="12">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="I169" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I169" s="12">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.15">
@@ -6447,49 +6493,127 @@
       <c r="D170" s="5">
         <v>3</v>
       </c>
+      <c r="E170" s="5">
+        <v>3</v>
+      </c>
       <c r="F170" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G170" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="H170" s="12">
+        <f t="shared" ref="H170:H233" si="22">IF(OR(D170="", E170=""), "", D170-E170)</f>
+        <v>0</v>
+      </c>
+      <c r="I170" s="12">
+        <f t="shared" ref="I170:I233" si="23">IF(OR(H170="",E170=0),"",ABS(H170)/E170*100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A171" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="B171" t="s">
+        <v>35</v>
+      </c>
+      <c r="C171" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D171" s="5">
+        <v>4</v>
+      </c>
+      <c r="E171" s="5">
+        <v>4</v>
+      </c>
+      <c r="F171" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G171" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="H171" s="12">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="I171" s="12">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A172" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B172" t="s">
+        <v>44</v>
+      </c>
+      <c r="C172" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D172" s="5">
+        <v>1</v>
+      </c>
+      <c r="E172" s="5">
+        <v>1</v>
+      </c>
+      <c r="F172" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H172" s="12">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="I172" s="12">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A173" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B173" t="s">
+        <v>156</v>
+      </c>
+      <c r="C173" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D173" s="5">
+        <v>4</v>
+      </c>
+      <c r="E173" s="5">
+        <v>3</v>
+      </c>
+      <c r="F173" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H173" s="12">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="I173" s="12">
+        <f t="shared" si="23"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A174" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B174" t="s">
+        <v>156</v>
+      </c>
+      <c r="C174" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D174" s="5">
+        <v>5</v>
+      </c>
+      <c r="F174" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H170" s="12" t="str">
-        <f t="shared" ref="H170:H233" si="22">IF(OR(D170="", E170=""), "", D170-E170)</f>
-        <v/>
-      </c>
-      <c r="I170" s="12" t="str">
-        <f t="shared" ref="I170:I233" si="23">IF(OR(H170="",E170=0),"",ABS(H170)/E170*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H171" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I171" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H172" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I172" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H173" s="12" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I173" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H174" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6500,6 +6624,21 @@
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A175" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B175" t="s">
+        <v>44</v>
+      </c>
+      <c r="C175" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D175" s="5">
+        <v>2</v>
+      </c>
+      <c r="F175" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H175" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6510,6 +6649,21 @@
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A176" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="B176" t="s">
+        <v>156</v>
+      </c>
+      <c r="C176" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="D176" s="5">
+        <v>6</v>
+      </c>
+      <c r="F176" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H176" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6519,7 +6673,16 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A177" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="B177" s="36"/>
+      <c r="C177" s="37"/>
+      <c r="D177" s="37"/>
+      <c r="E177" s="37"/>
+      <c r="F177" s="38"/>
+      <c r="G177" s="36"/>
       <c r="H177" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6529,7 +6692,19 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A178" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B178" t="s">
+        <v>156</v>
+      </c>
+      <c r="C178" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D178" s="5">
+        <v>2</v>
+      </c>
       <c r="H178" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6539,7 +6714,19 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A179" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B179" t="s">
+        <v>156</v>
+      </c>
+      <c r="C179" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D179" s="5">
+        <v>5</v>
+      </c>
       <c r="H179" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6549,7 +6736,19 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A180" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B180" t="s">
+        <v>44</v>
+      </c>
+      <c r="C180" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D180" s="5">
+        <v>2</v>
+      </c>
       <c r="H180" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6559,7 +6758,19 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A181" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="B181" t="s">
+        <v>156</v>
+      </c>
+      <c r="C181" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="D181" s="5">
+        <v>6</v>
+      </c>
       <c r="H181" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6569,7 +6780,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H182" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6579,7 +6790,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H183" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6589,7 +6800,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H184" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6599,7 +6810,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H185" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6609,7 +6820,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H186" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6619,7 +6830,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H187" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6629,7 +6840,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H188" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6639,7 +6850,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H189" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6649,7 +6860,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H190" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6659,7 +6870,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H191" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6669,7 +6880,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H192" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>

</xml_diff>

<commit_message>
Week 13 completed, Week 14 (Final Week) Planned
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/Project_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{471C2595-73D6-5B4F-B180-2232A1947209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06109003-FFE3-3742-8F7B-12BAE368BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="295">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -956,6 +956,69 @@
   </si>
   <si>
     <t>Week 13 (April 15-April 22)</t>
+  </si>
+  <si>
+    <t>Frame by frame asynchronous removed from requirement due to negligent change in performance,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On non GPU instance (c5.4x) the backend is running, and requests are also getting sent. </t>
+  </si>
+  <si>
+    <t>Client meeting-26</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-26</t>
+  </si>
+  <si>
+    <t>Client meeting-27</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-27</t>
+  </si>
+  <si>
+    <t>Client meeting-28</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-28</t>
+  </si>
+  <si>
+    <t>Video detected frames getting displayed on clicking the video, both from upload and live video</t>
+  </si>
+  <si>
+    <t>12-04-24: Final demo on AWS backend, and on running on non-GPU instance</t>
+  </si>
+  <si>
+    <t>Cost Analysis of GPU instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client requirede a costing analysis between GPU and non-GPU instance, and also about whether the current instance in documentation supports NVIDIA Drivers. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-04-24: Gave updates about the non-GPU instance throwing OSError of Less Memory, new hard coded CV Algo provided to be integrated in the current backend </t>
+  </si>
+  <si>
+    <t>08-04-24: Shown that the codebase is uploaded on AWS instance, asked us to start documenting the work that has been done by us.</t>
+  </si>
+  <si>
+    <t>Integrating new CV Algorithm</t>
+  </si>
+  <si>
+    <t>Final Documentation Client</t>
+  </si>
+  <si>
+    <t>Rohan S &amp; Rohan N</t>
+  </si>
+  <si>
+    <t>R2 Final Documentation</t>
+  </si>
+  <si>
+    <t>Rohan Sh &amp; Aanvik</t>
+  </si>
+  <si>
+    <t>Memory Analysis for NVIDIA Drivers</t>
+  </si>
+  <si>
+    <t>Week 14 (April 23-April 30)</t>
   </si>
 </sst>
 </file>
@@ -1828,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -6412,7 +6475,7 @@
       <c r="F167" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G167" s="42" t="s">
+      <c r="G167" s="29" t="s">
         <v>272</v>
       </c>
       <c r="H167" s="12">
@@ -6499,7 +6562,7 @@
       <c r="F170" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G170" s="42" t="s">
+      <c r="G170" s="29" t="s">
         <v>271</v>
       </c>
       <c r="H170" s="12">
@@ -6705,13 +6768,22 @@
       <c r="D178" s="5">
         <v>2</v>
       </c>
-      <c r="H178" s="12" t="str">
+      <c r="E178" s="5">
+        <v>2</v>
+      </c>
+      <c r="F178" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G178" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="H178" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I178" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I178" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.15">
@@ -6727,13 +6799,22 @@
       <c r="D179" s="5">
         <v>5</v>
       </c>
-      <c r="H179" s="12" t="str">
+      <c r="E179" s="5">
+        <v>5</v>
+      </c>
+      <c r="F179" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G179" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="H179" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I179" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I179" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.15">
@@ -6749,13 +6830,20 @@
       <c r="D180" s="5">
         <v>2</v>
       </c>
-      <c r="H180" s="12" t="str">
+      <c r="E180" s="5">
+        <v>1</v>
+      </c>
+      <c r="F180" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G180" s="29"/>
+      <c r="H180" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I180" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I180" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>100</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.15">
@@ -6771,96 +6859,279 @@
       <c r="D181" s="5">
         <v>6</v>
       </c>
-      <c r="H181" s="12" t="str">
+      <c r="E181" s="5">
+        <v>6</v>
+      </c>
+      <c r="F181" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G181" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="H181" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I181" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I181" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H182" s="12" t="str">
+      <c r="A182" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="B182" t="s">
+        <v>35</v>
+      </c>
+      <c r="C182" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D182" s="5">
+        <v>5</v>
+      </c>
+      <c r="E182" s="5">
+        <v>5</v>
+      </c>
+      <c r="F182" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G182" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="H182" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I182" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I182" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H183" s="12" t="str">
+      <c r="A183" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B183" t="s">
+        <v>44</v>
+      </c>
+      <c r="C183" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D183" s="5">
+        <v>1</v>
+      </c>
+      <c r="E183" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F183" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G183" s="29"/>
+      <c r="H183" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I183" s="12" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="I183" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H184" s="12" t="str">
+      <c r="A184" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B184" t="s">
+        <v>35</v>
+      </c>
+      <c r="C184" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D184" s="5">
+        <v>5</v>
+      </c>
+      <c r="E184" s="5">
+        <v>5</v>
+      </c>
+      <c r="F184" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G184" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="H184" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I184" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I184" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H185" s="12" t="str">
+      <c r="A185" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B185" t="s">
+        <v>44</v>
+      </c>
+      <c r="C185" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D185" s="5">
+        <v>1</v>
+      </c>
+      <c r="E185" s="5">
+        <v>1</v>
+      </c>
+      <c r="F185" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G185" s="29"/>
+      <c r="H185" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I185" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I185" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H186" s="12" t="str">
+      <c r="A186" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B186" t="s">
+        <v>35</v>
+      </c>
+      <c r="C186" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D186" s="5">
+        <v>5</v>
+      </c>
+      <c r="E186" s="5">
+        <v>5</v>
+      </c>
+      <c r="F186" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G186" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="H186" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I186" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I186" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H187" s="12" t="str">
+      <c r="A187" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B187" t="s">
+        <v>44</v>
+      </c>
+      <c r="C187" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D187" s="5">
+        <v>1</v>
+      </c>
+      <c r="E187" s="5">
+        <v>1</v>
+      </c>
+      <c r="F187" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G187" s="29"/>
+      <c r="H187" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I187" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I187" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H188" s="12" t="str">
+      <c r="A188" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="B188" t="s">
+        <v>38</v>
+      </c>
+      <c r="C188" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D188" s="5">
+        <v>2</v>
+      </c>
+      <c r="E188" s="5">
+        <v>2</v>
+      </c>
+      <c r="F188" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G188" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="H188" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I188" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I188" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H189" s="12" t="str">
+      <c r="A189" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="B189" t="s">
+        <v>156</v>
+      </c>
+      <c r="C189" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D189" s="5">
+        <v>4</v>
+      </c>
+      <c r="E189" s="5">
+        <v>2</v>
+      </c>
+      <c r="F189" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H189" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I189" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="I189" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>100</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A190" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="B190" t="s">
+        <v>44</v>
+      </c>
+      <c r="C190" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="D190" s="5">
+        <v>6</v>
+      </c>
+      <c r="F190" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H190" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6871,6 +7142,21 @@
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A191" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="B191" t="s">
+        <v>44</v>
+      </c>
+      <c r="C191" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="D191" s="5">
+        <v>6</v>
+      </c>
+      <c r="F191" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H191" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6881,6 +7167,21 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A192" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="B192" t="s">
+        <v>38</v>
+      </c>
+      <c r="C192" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D192" s="5">
+        <v>4</v>
+      </c>
+      <c r="F192" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="H192" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6890,7 +7191,16 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A193" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B193" s="36"/>
+      <c r="C193" s="37"/>
+      <c r="D193" s="37"/>
+      <c r="E193" s="37"/>
+      <c r="F193" s="38"/>
+      <c r="G193" s="36"/>
       <c r="H193" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6900,7 +7210,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H194" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6910,7 +7220,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H195" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6920,7 +7230,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H196" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6930,7 +7240,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H197" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6940,7 +7250,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H198" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6950,7 +7260,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H199" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6960,7 +7270,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H200" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6970,7 +7280,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H201" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6980,7 +7290,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H202" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6990,7 +7300,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H203" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7000,7 +7310,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H204" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7010,7 +7320,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H205" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7020,7 +7330,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H206" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7030,7 +7340,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H207" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7040,7 +7350,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H208" s="12" t="str">
         <f t="shared" si="22"/>
         <v/>

</xml_diff>

<commit_message>
Week 14 completed, completing the Status Tracker
</commit_message>
<xml_diff>
--- a/StatusTracker_Team33.xlsx
+++ b/StatusTracker_Team33.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aanvikbhatnagar/Desktop/DASS-S24/Project_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06109003-FFE3-3742-8F7B-12BAE368BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3102D118-0AE7-724A-B6E5-F5709D02C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="315">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -1006,9 +1006,6 @@
     <t>Final Documentation Client</t>
   </si>
   <si>
-    <t>Rohan S &amp; Rohan N</t>
-  </si>
-  <si>
     <t>R2 Final Documentation</t>
   </si>
   <si>
@@ -1019,6 +1016,69 @@
   </si>
   <si>
     <t>Week 14 (April 23-April 30)</t>
+  </si>
+  <si>
+    <t>Client meeting-29</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-29</t>
+  </si>
+  <si>
+    <t>Client meeting-30</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-30</t>
+  </si>
+  <si>
+    <t>Final Video Demo Recording</t>
+  </si>
+  <si>
+    <t>Client meeting-31</t>
+  </si>
+  <si>
+    <t>MoM Client Meet-31</t>
+  </si>
+  <si>
+    <t>APK Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows Deployment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 Presentation </t>
+  </si>
+  <si>
+    <t>Rohan Sh &amp; Chetan &amp; Aanvik</t>
+  </si>
+  <si>
+    <t>Aanvik &amp; Rohan N</t>
+  </si>
+  <si>
+    <t>AWS Deployment: Aanvik, Quick Startup: Chetan, Workflow: Rohan Sh</t>
+  </si>
+  <si>
+    <t>Updating all the versions of all documents based on the final requirements and outcomes of the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client asked how much memory is needed for NVIDIA Drivers to be installed, and what is the procedure for the same. </t>
+  </si>
+  <si>
+    <t>15-04-24: Discussed about closing plans of the project, and documentation regarding all the work needs to get started</t>
+  </si>
+  <si>
+    <t>17-04-24: Discussed about GPU instance, deployment of updated CV algorithm on AWS, and Windows set up for the codebase</t>
+  </si>
+  <si>
+    <t>Final work distribution for documentation and R2 related presentation work discussed. Wrap up the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19-04-24: Meet with the CEO, client testing the app across network, final comments about the project </t>
+  </si>
+  <si>
+    <t>Removing the dependency of Expo Go keeping the network same for both host and mobile, to APK for bundling across networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration of Windows for frontend and backend codebase set up. </t>
   </si>
 </sst>
 </file>
@@ -1401,6 +1461,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1891,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E212" sqref="E212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -6774,7 +6838,7 @@
       <c r="F178" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G178" s="42" t="s">
+      <c r="G178" s="29" t="s">
         <v>275</v>
       </c>
       <c r="H178" s="12">
@@ -6805,7 +6869,7 @@
       <c r="F179" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G179" s="42" t="s">
+      <c r="G179" s="29" t="s">
         <v>274</v>
       </c>
       <c r="H179" s="12">
@@ -7016,7 +7080,7 @@
       <c r="F186" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G186" s="42" t="s">
+      <c r="G186" s="29" t="s">
         <v>283</v>
       </c>
       <c r="H186" s="12">
@@ -7076,7 +7140,7 @@
       <c r="F188" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G188" s="42" t="s">
+      <c r="G188" s="29" t="s">
         <v>285</v>
       </c>
       <c r="H188" s="12">
@@ -7123,8 +7187,8 @@
       <c r="B190" t="s">
         <v>44</v>
       </c>
-      <c r="C190" s="31" t="s">
-        <v>290</v>
+      <c r="C190" s="35" t="s">
+        <v>304</v>
       </c>
       <c r="D190" s="5">
         <v>6</v>
@@ -7143,13 +7207,13 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A191" s="32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B191" t="s">
         <v>44</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D191" s="5">
         <v>6</v>
@@ -7168,7 +7232,7 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A192" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B192" t="s">
         <v>38</v>
@@ -7193,7 +7257,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A193" s="39" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B193" s="36"/>
       <c r="C193" s="37"/>
@@ -7211,143 +7275,427 @@
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H194" s="12" t="str">
+      <c r="A194" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="B194" t="s">
+        <v>44</v>
+      </c>
+      <c r="C194" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="D194" s="5">
+        <v>6</v>
+      </c>
+      <c r="E194" s="5">
+        <v>6</v>
+      </c>
+      <c r="F194" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G194" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="H194" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I194" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I194" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H195" s="12" t="str">
+      <c r="A195" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="B195" t="s">
+        <v>44</v>
+      </c>
+      <c r="C195" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D195" s="5">
+        <v>6</v>
+      </c>
+      <c r="E195" s="5">
+        <v>6</v>
+      </c>
+      <c r="F195" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G195" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="H195" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I195" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I195" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H196" s="12" t="str">
+      <c r="A196" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="B196" t="s">
+        <v>38</v>
+      </c>
+      <c r="C196" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D196" s="5">
+        <v>4</v>
+      </c>
+      <c r="E196" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="F196" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G196" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="H196" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I196" s="12" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="I196" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H197" s="12" t="str">
+      <c r="A197" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B197" t="s">
+        <v>35</v>
+      </c>
+      <c r="C197" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D197" s="5">
+        <v>5</v>
+      </c>
+      <c r="E197" s="5">
+        <v>5</v>
+      </c>
+      <c r="F197" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G197" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="H197" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I197" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I197" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H198" s="12" t="str">
+      <c r="A198" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="B198" t="s">
+        <v>44</v>
+      </c>
+      <c r="C198" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D198" s="5">
+        <v>1</v>
+      </c>
+      <c r="E198" s="5">
+        <v>1</v>
+      </c>
+      <c r="F198" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G198" s="29"/>
+      <c r="H198" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I198" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I198" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H199" s="12" t="str">
+      <c r="A199" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="B199" t="s">
+        <v>35</v>
+      </c>
+      <c r="C199" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D199" s="5">
+        <v>5</v>
+      </c>
+      <c r="E199" s="5">
+        <v>5</v>
+      </c>
+      <c r="F199" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G199" s="42" t="s">
+        <v>310</v>
+      </c>
+      <c r="H199" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I199" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I199" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H200" s="12" t="str">
+      <c r="A200" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="B200" t="s">
+        <v>44</v>
+      </c>
+      <c r="C200" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D200" s="5">
+        <v>1</v>
+      </c>
+      <c r="E200" s="5">
+        <v>1</v>
+      </c>
+      <c r="F200" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G200" s="29"/>
+      <c r="H200" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I200" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I200" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H201" s="12" t="str">
+      <c r="A201" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B201" t="s">
+        <v>35</v>
+      </c>
+      <c r="C201" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D201" s="5">
+        <v>2</v>
+      </c>
+      <c r="E201" s="5">
+        <v>2</v>
+      </c>
+      <c r="F201" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G201" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="H201" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I201" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I201" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H202" s="12" t="str">
+      <c r="A202" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B202" t="s">
+        <v>141</v>
+      </c>
+      <c r="C202" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="D202" s="5">
+        <v>4</v>
+      </c>
+      <c r="E202" s="5">
+        <v>4</v>
+      </c>
+      <c r="F202" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G202" s="29"/>
+      <c r="H202" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I202" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I202" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H203" s="12" t="str">
+      <c r="A203" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="B203" t="s">
+        <v>35</v>
+      </c>
+      <c r="C203" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D203" s="5">
+        <v>6</v>
+      </c>
+      <c r="E203" s="5">
+        <v>6</v>
+      </c>
+      <c r="F203" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G203" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="H203" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I203" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I203" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H204" s="12" t="str">
+      <c r="A204" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="B204" t="s">
+        <v>44</v>
+      </c>
+      <c r="C204" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D204" s="5">
+        <v>1</v>
+      </c>
+      <c r="E204" s="5">
+        <v>1</v>
+      </c>
+      <c r="F204" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G204" s="29"/>
+      <c r="H204" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I204" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I204" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H205" s="12" t="str">
+      <c r="A205" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="B205" t="s">
+        <v>156</v>
+      </c>
+      <c r="C205" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D205" s="5">
+        <v>4</v>
+      </c>
+      <c r="E205" s="5">
+        <v>4</v>
+      </c>
+      <c r="F205" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G205" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="H205" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I205" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I205" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H206" s="12" t="str">
+      <c r="A206" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="B206" t="s">
+        <v>156</v>
+      </c>
+      <c r="C206" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D206" s="5">
+        <v>2</v>
+      </c>
+      <c r="E206" s="5">
+        <v>2</v>
+      </c>
+      <c r="F206" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G206" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="H206" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I206" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I206" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H207" s="12" t="str">
+      <c r="A207" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B207" t="s">
+        <v>44</v>
+      </c>
+      <c r="C207" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="D207" s="5">
+        <v>5</v>
+      </c>
+      <c r="E207" s="5">
+        <v>5</v>
+      </c>
+      <c r="F207" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G207" s="29"/>
+      <c r="H207" s="12">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="I207" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I207" s="12">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>